<commit_message>
Corrección del diagrama de clases
</commit_message>
<xml_diff>
--- a/Desarrollo/SGDS/Gestion/SGDS-CP.xlsx
+++ b/Desarrollo/SGDS/Gestion/SGDS-CP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Backup\Escritorio\QuantumAnts Software\QuantumAnts-Software\Desarrollo\SGDS\Gestion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Proyecto_Grupo_5\QuantumAnts-Software\Desarrollo\SGDS\Gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D822574-0B8F-46D6-8D19-86C99A1782C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEDA21C2-5011-4FCA-87E8-F4B1D63AE7D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma #1" sheetId="1" r:id="rId1"/>
@@ -1913,8 +1913,8 @@
   </sheetPr>
   <dimension ref="A1:K998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -2666,8 +2666,8 @@
       <c r="D32" s="105" t="s">
         <v>169</v>
       </c>
-      <c r="E32" s="32" t="s">
-        <v>33</v>
+      <c r="E32" s="29" t="s">
+        <v>36</v>
       </c>
       <c r="F32" s="36">
         <v>45061</v>

</xml_diff>

<commit_message>
Actualización del Cronograma y Documento de Sprint Retrospective creado
</commit_message>
<xml_diff>
--- a/Desarrollo/SGDS/Gestion/SGDS-CP.xlsx
+++ b/Desarrollo/SGDS/Gestion/SGDS-CP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Proyecto_Grupo_5\QuantumAnts-Software\Desarrollo\SGDS\Gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCCAF36-25C5-40C7-AC4C-B754FCD925F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C18143D-231A-4288-BEDB-8015FCC911BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1969,7 +1969,7 @@
   <dimension ref="A1:K998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="B31" sqref="B31:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Agregando archivos alinea base 2
</commit_message>
<xml_diff>
--- a/Desarrollo/SGDS/Gestion/SGDS-CP.xlsx
+++ b/Desarrollo/SGDS/Gestion/SGDS-CP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Proyecto_Grupo_5\QuantumAnts-Software\Desarrollo\SGDS\Gestion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Backup\Escritorio\QuantumAnts Software\QuantumAnts-Software\Desarrollo\SGDS\Gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731509B0-1975-40BD-8670-7030AC0F69D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51AD4B9-30DB-4799-95F0-0D7735A221EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma #1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="186">
   <si>
     <t>CRONOGRAMA DEL PROYECTO</t>
   </si>
@@ -690,6 +690,21 @@
   </si>
   <si>
     <t>SGDS.RDS-03.DOCX</t>
+  </si>
+  <si>
+    <r>
+      <t>SGDS-</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF5AADF1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>IVUI.html</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1968,8 +1983,8 @@
   </sheetPr>
   <dimension ref="A1:K998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C11" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -2800,7 +2815,7 @@
         <v>168</v>
       </c>
       <c r="D35" s="101" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="E35" s="48" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
Plan actualizado y cronograma actualizado
</commit_message>
<xml_diff>
--- a/Desarrollo/SGDS/Gestion/SGDS-CP.xlsx
+++ b/Desarrollo/SGDS/Gestion/SGDS-CP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Backup\Escritorio\QuantumAnts Software\QuantumAnts-Software\Desarrollo\SGDS\Gestion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Proyecto_Grupo_5\QuantumAnts-Software\Desarrollo\SGDS\Gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51AD4B9-30DB-4799-95F0-0D7735A221EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C52727-216A-44DF-BBCE-00AE962C7584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12690" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma #1" sheetId="1" r:id="rId1"/>
@@ -1983,8 +1983,8 @@
   </sheetPr>
   <dimension ref="A1:K998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40:H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -2959,7 +2959,7 @@
         <v>45087</v>
       </c>
       <c r="H40" s="52">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I40" s="21"/>
       <c r="J40" s="46"/>
@@ -2986,7 +2986,7 @@
         <v>45087</v>
       </c>
       <c r="H41" s="52">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I41" s="21"/>
       <c r="J41" s="46"/>
@@ -3013,7 +3013,7 @@
         <v>45087</v>
       </c>
       <c r="H42" s="52">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I42" s="21"/>
       <c r="J42" s="46"/>
@@ -3040,7 +3040,7 @@
         <v>45087</v>
       </c>
       <c r="H43" s="52">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I43" s="21"/>
       <c r="J43" s="46"/>
@@ -3067,7 +3067,7 @@
         <v>45087</v>
       </c>
       <c r="H44" s="52">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I44" s="21"/>
       <c r="J44" s="46"/>
@@ -3313,7 +3313,7 @@
       </c>
       <c r="H53" s="64">
         <f>SUM(H40:H52)/13</f>
-        <v>0</v>
+        <v>0.19230769230769232</v>
       </c>
       <c r="I53" s="111"/>
     </row>

</xml_diff>

<commit_message>
Plan corregido y cronograma actualizado
</commit_message>
<xml_diff>
--- a/Desarrollo/SGDS/Gestion/SGDS-CP.xlsx
+++ b/Desarrollo/SGDS/Gestion/SGDS-CP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Proyecto_Grupo_5\QuantumAnts-Software\Desarrollo\SGDS\Gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C52727-216A-44DF-BBCE-00AE962C7584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF5D2B6-EFD0-428B-AE2C-5866591614EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12690" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1983,8 +1983,8 @@
   </sheetPr>
   <dimension ref="A1:K998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40:H44"/>
+    <sheetView tabSelected="1" topLeftCell="C18" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -2636,7 +2636,7 @@
         <v>45053</v>
       </c>
       <c r="G28" s="31">
-        <v>45087</v>
+        <v>45056</v>
       </c>
       <c r="H28" s="20">
         <v>1</v>

</xml_diff>

<commit_message>
Cronograma actualizado y finalizado
</commit_message>
<xml_diff>
--- a/Desarrollo/SGDS/Gestion/SGDS-CP.xlsx
+++ b/Desarrollo/SGDS/Gestion/SGDS-CP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Proyecto_Grupo_5\QuantumAnts-Software\Desarrollo\SGDS\Gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85B2EEB-107C-419E-B553-02FE38C91B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43368DDB-B526-462C-BE27-B2D2C2C7E962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1983,8 +1983,8 @@
   </sheetPr>
   <dimension ref="A1:K998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D34" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="D31" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -3287,7 +3287,7 @@
         <v>45095</v>
       </c>
       <c r="H52" s="52">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="I52" s="111"/>
       <c r="J52" s="46"/>
@@ -3313,7 +3313,7 @@
       </c>
       <c r="H53" s="64">
         <f>SUM(H40:H52)/13</f>
-        <v>0.9538461538461539</v>
+        <v>1</v>
       </c>
       <c r="I53" s="111"/>
     </row>

</xml_diff>

<commit_message>
Implementando el requisito 04
</commit_message>
<xml_diff>
--- a/Desarrollo/SGDS/Gestion/SGDS-CP.xlsx
+++ b/Desarrollo/SGDS/Gestion/SGDS-CP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Proyecto_Grupo_5\QuantumAnts-Software\Desarrollo\SGDS\Gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85B2EEB-107C-419E-B553-02FE38C91B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43368DDB-B526-462C-BE27-B2D2C2C7E962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1983,8 +1983,8 @@
   </sheetPr>
   <dimension ref="A1:K998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D34" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="D31" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -3287,7 +3287,7 @@
         <v>45095</v>
       </c>
       <c r="H52" s="52">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="I52" s="111"/>
       <c r="J52" s="46"/>
@@ -3313,7 +3313,7 @@
       </c>
       <c r="H53" s="64">
         <f>SUM(H40:H52)/13</f>
-        <v>0.9538461538461539</v>
+        <v>1</v>
       </c>
       <c r="I53" s="111"/>
     </row>

</xml_diff>

<commit_message>
Corrigiendo nomenclatura de implementacion de requisitos 8 y 9
</commit_message>
<xml_diff>
--- a/Desarrollo/SGDS/Gestion/SGDS-CP.xlsx
+++ b/Desarrollo/SGDS/Gestion/SGDS-CP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Proyecto_Grupo_5\QuantumAnts-Software\Desarrollo\SGDS\Gestion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Backup\Escritorio\QuantumAnts Software\QuantumAnts-Software\Desarrollo\SGDS\Gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43368DDB-B526-462C-BE27-B2D2C2C7E962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E7A7BB-5905-4B4B-ACD7-7DC004B3529D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma #1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="185">
   <si>
     <t>CRONOGRAMA DEL PROYECTO</t>
   </si>
@@ -648,30 +648,6 @@
   </si>
   <si>
     <t>SGDS-DER09.DOCX</t>
-  </si>
-  <si>
-    <r>
-      <t>SGDS-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF5AADF1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>IVUI.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>js</t>
-    </r>
   </si>
   <si>
     <t>Verificación y Actualización de la Base de Datos 01</t>
@@ -1983,8 +1959,8 @@
   </sheetPr>
   <dimension ref="A1:K998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D31" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -2761,7 +2737,7 @@
         <v>164</v>
       </c>
       <c r="D33" s="100" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E33" s="29" t="s">
         <v>39</v>
@@ -2815,7 +2791,7 @@
         <v>168</v>
       </c>
       <c r="D35" s="101" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E35" s="48" t="s">
         <v>61</v>
@@ -2869,7 +2845,7 @@
         <v>67</v>
       </c>
       <c r="D37" s="102" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E37" s="48" t="s">
         <v>65</v>
@@ -3106,7 +3082,7 @@
         <v>82</v>
       </c>
       <c r="C46" s="44" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D46" s="98" t="s">
         <v>151</v>
@@ -3136,7 +3112,7 @@
         <v>168</v>
       </c>
       <c r="D47" s="101" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="E47" s="48" t="s">
         <v>61</v>
@@ -3187,10 +3163,10 @@
         <v>84</v>
       </c>
       <c r="C49" s="47" t="s">
+        <v>179</v>
+      </c>
+      <c r="D49" s="98" t="s">
         <v>180</v>
-      </c>
-      <c r="D49" s="98" t="s">
-        <v>181</v>
       </c>
       <c r="E49" s="48" t="s">
         <v>48</v>
@@ -3219,7 +3195,7 @@
         <v>67</v>
       </c>
       <c r="D50" s="102" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E50" s="48" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
Cronograma de implementación de la solicitud de cambio creada y documento del Plan de la Gestión de la Configuración modificada
</commit_message>
<xml_diff>
--- a/Desarrollo/SGDS/Gestion/SGDS-CP.xlsx
+++ b/Desarrollo/SGDS/Gestion/SGDS-CP.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Backup\Escritorio\QuantumAnts Software\QuantumAnts-Software\Desarrollo\SGDS\Gestion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Proyecto_Grupo_5\QuantumAnts-Software\Desarrollo\SGDS\Gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E7A7BB-5905-4B4B-ACD7-7DC004B3529D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF217E9-C429-4C30-87FE-7F076AB73B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma #1" sheetId="1" r:id="rId1"/>
-    <sheet name="IntegrantesRoles" sheetId="2" r:id="rId2"/>
-    <sheet name="Ideas de requisitos" sheetId="3" r:id="rId3"/>
+    <sheet name="Cronograma#2" sheetId="4" r:id="rId2"/>
+    <sheet name="IntegrantesRoles" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="185">
   <si>
     <t>CRONOGRAMA DEL PROYECTO</t>
   </si>
@@ -360,66 +360,6 @@
   </si>
   <si>
     <t>Designer UI (DU) / Programador Frontend (PF)</t>
-  </si>
-  <si>
-    <t>Requisitos</t>
-  </si>
-  <si>
-    <t>Jatziry</t>
-  </si>
-  <si>
-    <t>Jose</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Fabricio</t>
-  </si>
-  <si>
-    <t>Funcionales</t>
-  </si>
-  <si>
-    <t>No Funcionales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Registro de hospitales </t>
-  </si>
-  <si>
-    <t>Geomar</t>
-  </si>
-  <si>
-    <t>Renzo</t>
-  </si>
-  <si>
-    <t>Registro de donantes</t>
-  </si>
-  <si>
-    <t>Programación de citas</t>
-  </si>
-  <si>
-    <t>Registro de donaciones</t>
-  </si>
-  <si>
-    <t>Entrega de beneficios</t>
-  </si>
-  <si>
-    <t>Validación de beneficios</t>
-  </si>
-  <si>
-    <t>Reportes y estadísticas</t>
-  </si>
-  <si>
-    <t>Seguridad de la información</t>
-  </si>
-  <si>
-    <t>Accesibilidad</t>
-  </si>
-  <si>
-    <t>Integración con sistemas existentes</t>
-  </si>
-  <si>
-    <t>Registro de Solicitantes</t>
   </si>
   <si>
     <t>SGDS-DAS01.DOCX</t>
@@ -682,12 +622,72 @@
       <t>IVUI.html</t>
     </r>
   </si>
+  <si>
+    <t>CRONOGRAMA DEL PROYECTO - SC014</t>
+  </si>
+  <si>
+    <t>Modificar el Plan de Proyecto</t>
+  </si>
+  <si>
+    <t>Elaborar Cronograma de la Solicitud de Cambio</t>
+  </si>
+  <si>
+    <t>Actualizar el Documento de Arquitectura de Software</t>
+  </si>
+  <si>
+    <t>Actualizar el Documento de Guia de Estilos</t>
+  </si>
+  <si>
+    <t>Actualizar el Documento de Especificación de la Base de Datos</t>
+  </si>
+  <si>
+    <t>Actualizar el Documento del Requisito 08: Registro de donante</t>
+  </si>
+  <si>
+    <t>Actualizar el Documento de Especificación de UI</t>
+  </si>
+  <si>
+    <t>Saavedra M. (JP/AS)</t>
+  </si>
+  <si>
+    <t>Proceso de Script 1</t>
+  </si>
+  <si>
+    <t>Proceso de Script 2</t>
+  </si>
+  <si>
+    <t>Proceso de Script 3</t>
+  </si>
+  <si>
+    <t>Actualización de la Base de Datos</t>
+  </si>
+  <si>
+    <t>Implemenctación de la Interfaz Web</t>
+  </si>
+  <si>
+    <t>Elaborar del acta de cierre de la solicitud del proyecto</t>
+  </si>
+  <si>
+    <t>SGDS-PS-SC014.py</t>
+  </si>
+  <si>
+    <t>Acta de Cierre de la Solicitud de Cambio 14 del Proyecto</t>
+  </si>
+  <si>
+    <t>PGC</t>
+  </si>
+  <si>
+    <t>Documento del Plan de la Gestión de la Configuración</t>
+  </si>
+  <si>
+    <t>SGDS-ACP-SC014.DOCX</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="51">
+  <fonts count="42">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -887,59 +887,6 @@
       <name val="Montserrat"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFF9900"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF4A86E8"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFF00AA"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF38761D"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF3D85C6"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
@@ -1498,7 +1445,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1661,70 +1608,98 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="7" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="43" fillId="7" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="27" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1955,12 +1930,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
+    <tabColor theme="7"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:K998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -2051,7 +2027,7 @@
         <v>45022</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="104"/>
+      <c r="E6" s="83"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="4"/>
@@ -2088,7 +2064,7 @@
       <c r="C9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="97" t="s">
+      <c r="D9" s="76" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="14" t="s">
@@ -2114,7 +2090,7 @@
       <c r="C10" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="98" t="s">
+      <c r="D10" s="77" t="s">
         <v>18</v>
       </c>
       <c r="E10" s="18" t="s">
@@ -2140,7 +2116,7 @@
       <c r="C11" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="98" t="s">
+      <c r="D11" s="77" t="s">
         <v>18</v>
       </c>
       <c r="E11" s="18" t="s">
@@ -2168,8 +2144,8 @@
       <c r="C12" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="98" t="s">
-        <v>137</v>
+      <c r="D12" s="77" t="s">
+        <v>117</v>
       </c>
       <c r="E12" s="18" t="s">
         <v>19</v>
@@ -2197,8 +2173,8 @@
       <c r="C13" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="98" t="s">
-        <v>138</v>
+      <c r="D13" s="77" t="s">
+        <v>118</v>
       </c>
       <c r="E13" s="29" t="s">
         <v>27</v>
@@ -2223,7 +2199,7 @@
       <c r="C14" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="98" t="s">
+      <c r="D14" s="77" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="29" t="s">
@@ -2249,8 +2225,8 @@
       <c r="C15" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="98" t="s">
-        <v>169</v>
+      <c r="D15" s="77" t="s">
+        <v>149</v>
       </c>
       <c r="E15" s="32" t="s">
         <v>33</v>
@@ -2276,8 +2252,8 @@
       <c r="C16" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="98" t="s">
-        <v>170</v>
+      <c r="D16" s="77" t="s">
+        <v>150</v>
       </c>
       <c r="E16" s="29" t="s">
         <v>36</v>
@@ -2303,8 +2279,8 @@
       <c r="C17" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="98" t="s">
-        <v>171</v>
+      <c r="D17" s="77" t="s">
+        <v>151</v>
       </c>
       <c r="E17" s="29" t="s">
         <v>39</v>
@@ -2330,8 +2306,8 @@
       <c r="C18" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="98" t="s">
-        <v>172</v>
+      <c r="D18" s="77" t="s">
+        <v>152</v>
       </c>
       <c r="E18" s="29" t="s">
         <v>39</v>
@@ -2357,11 +2333,11 @@
       <c r="C19" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="98" t="s">
-        <v>173</v>
+      <c r="D19" s="77" t="s">
+        <v>153</v>
       </c>
       <c r="E19" s="32" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="F19" s="24">
         <v>45033</v>
@@ -2384,11 +2360,11 @@
       <c r="C20" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="98" t="s">
-        <v>174</v>
+      <c r="D20" s="77" t="s">
+        <v>154</v>
       </c>
       <c r="E20" s="32" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="F20" s="24">
         <v>45033</v>
@@ -2411,8 +2387,8 @@
       <c r="C21" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="98" t="s">
-        <v>175</v>
+      <c r="D21" s="77" t="s">
+        <v>155</v>
       </c>
       <c r="E21" s="29" t="s">
         <v>48</v>
@@ -2438,8 +2414,8 @@
       <c r="C22" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="98" t="s">
-        <v>176</v>
+      <c r="D22" s="77" t="s">
+        <v>156</v>
       </c>
       <c r="E22" s="32" t="s">
         <v>30</v>
@@ -2465,8 +2441,8 @@
       <c r="C23" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="98" t="s">
-        <v>177</v>
+      <c r="D23" s="77" t="s">
+        <v>157</v>
       </c>
       <c r="E23" s="32" t="s">
         <v>30</v>
@@ -2492,8 +2468,8 @@
       <c r="C24" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="98" t="s">
-        <v>128</v>
+      <c r="D24" s="77" t="s">
+        <v>108</v>
       </c>
       <c r="E24" s="29" t="s">
         <v>55</v>
@@ -2519,8 +2495,8 @@
       <c r="C25" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="D25" s="98" t="s">
-        <v>129</v>
+      <c r="D25" s="77" t="s">
+        <v>109</v>
       </c>
       <c r="E25" s="29" t="s">
         <v>58</v>
@@ -2546,8 +2522,8 @@
       <c r="C26" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="98" t="s">
-        <v>139</v>
+      <c r="D26" s="77" t="s">
+        <v>119</v>
       </c>
       <c r="E26" s="29" t="s">
         <v>61</v>
@@ -2575,8 +2551,8 @@
       <c r="C27" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="D27" s="98" t="s">
-        <v>155</v>
+      <c r="D27" s="77" t="s">
+        <v>135</v>
       </c>
       <c r="E27" s="29" t="s">
         <v>65</v>
@@ -2602,8 +2578,8 @@
       <c r="C28" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="D28" s="98" t="s">
-        <v>154</v>
+      <c r="D28" s="77" t="s">
+        <v>134</v>
       </c>
       <c r="E28" s="29" t="s">
         <v>65</v>
@@ -2631,8 +2607,8 @@
       <c r="C29" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="D29" s="98" t="s">
-        <v>140</v>
+      <c r="D29" s="77" t="s">
+        <v>120</v>
       </c>
       <c r="E29" s="29" t="s">
         <v>48</v>
@@ -2658,7 +2634,7 @@
         <v>72</v>
       </c>
       <c r="C30" s="39"/>
-      <c r="D30" s="99"/>
+      <c r="D30" s="78"/>
       <c r="E30" s="40"/>
       <c r="F30" s="41">
         <v>45052</v>
@@ -2678,10 +2654,10 @@
         <v>73</v>
       </c>
       <c r="C31" s="44" t="s">
-        <v>162</v>
-      </c>
-      <c r="D31" s="100" t="s">
-        <v>141</v>
+        <v>142</v>
+      </c>
+      <c r="D31" s="79" t="s">
+        <v>121</v>
       </c>
       <c r="E31" s="32" t="s">
         <v>33</v>
@@ -2707,10 +2683,10 @@
         <v>75</v>
       </c>
       <c r="C32" s="44" t="s">
-        <v>163</v>
-      </c>
-      <c r="D32" s="100" t="s">
-        <v>142</v>
+        <v>143</v>
+      </c>
+      <c r="D32" s="79" t="s">
+        <v>122</v>
       </c>
       <c r="E32" s="29" t="s">
         <v>36</v>
@@ -2734,10 +2710,10 @@
         <v>76</v>
       </c>
       <c r="C33" s="44" t="s">
-        <v>164</v>
-      </c>
-      <c r="D33" s="100" t="s">
-        <v>181</v>
+        <v>144</v>
+      </c>
+      <c r="D33" s="79" t="s">
+        <v>161</v>
       </c>
       <c r="E33" s="29" t="s">
         <v>39</v>
@@ -2758,13 +2734,13 @@
     <row r="34" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A34" s="9"/>
       <c r="B34" s="43" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="C34" s="44" t="s">
-        <v>165</v>
-      </c>
-      <c r="D34" s="101" t="s">
-        <v>143</v>
+        <v>145</v>
+      </c>
+      <c r="D34" s="80" t="s">
+        <v>123</v>
       </c>
       <c r="E34" s="32" t="s">
         <v>33</v>
@@ -2785,13 +2761,13 @@
     <row r="35" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A35" s="9"/>
       <c r="B35" s="43" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="C35" s="47" t="s">
-        <v>168</v>
-      </c>
-      <c r="D35" s="101" t="s">
-        <v>184</v>
+        <v>148</v>
+      </c>
+      <c r="D35" s="80" t="s">
+        <v>164</v>
       </c>
       <c r="E35" s="48" t="s">
         <v>61</v>
@@ -2817,8 +2793,8 @@
       <c r="C36" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="D36" s="98" t="s">
-        <v>139</v>
+      <c r="D36" s="77" t="s">
+        <v>119</v>
       </c>
       <c r="E36" s="48" t="s">
         <v>61</v>
@@ -2844,8 +2820,8 @@
       <c r="C37" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="D37" s="102" t="s">
-        <v>182</v>
+      <c r="D37" s="81" t="s">
+        <v>162</v>
       </c>
       <c r="E37" s="48" t="s">
         <v>65</v>
@@ -2873,8 +2849,8 @@
       <c r="C38" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="D38" s="98" t="s">
-        <v>144</v>
+      <c r="D38" s="77" t="s">
+        <v>124</v>
       </c>
       <c r="E38" s="29" t="s">
         <v>48</v>
@@ -2899,8 +2875,8 @@
       <c r="B39" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="C39" s="107"/>
-      <c r="D39" s="99"/>
+      <c r="C39" s="86"/>
+      <c r="D39" s="78"/>
       <c r="E39" s="54"/>
       <c r="F39" s="55">
         <v>45061</v>
@@ -2916,14 +2892,14 @@
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A40" s="9"/>
-      <c r="B40" s="105" t="s">
-        <v>130</v>
-      </c>
-      <c r="C40" s="109" t="s">
-        <v>156</v>
-      </c>
-      <c r="D40" s="106" t="s">
-        <v>145</v>
+      <c r="B40" s="84" t="s">
+        <v>110</v>
+      </c>
+      <c r="C40" s="88" t="s">
+        <v>136</v>
+      </c>
+      <c r="D40" s="85" t="s">
+        <v>125</v>
       </c>
       <c r="E40" s="29" t="s">
         <v>39</v>
@@ -2943,17 +2919,17 @@
     </row>
     <row r="41" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A41" s="9"/>
-      <c r="B41" s="105" t="s">
-        <v>131</v>
-      </c>
-      <c r="C41" s="109" t="s">
-        <v>157</v>
-      </c>
-      <c r="D41" s="106" t="s">
-        <v>146</v>
+      <c r="B41" s="84" t="s">
+        <v>111</v>
+      </c>
+      <c r="C41" s="88" t="s">
+        <v>137</v>
+      </c>
+      <c r="D41" s="85" t="s">
+        <v>126</v>
       </c>
       <c r="E41" s="32" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="F41" s="36">
         <v>45078</v>
@@ -2970,17 +2946,17 @@
     </row>
     <row r="42" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A42" s="9"/>
-      <c r="B42" s="105" t="s">
-        <v>132</v>
-      </c>
-      <c r="C42" s="109" t="s">
-        <v>158</v>
-      </c>
-      <c r="D42" s="106" t="s">
-        <v>147</v>
+      <c r="B42" s="84" t="s">
+        <v>112</v>
+      </c>
+      <c r="C42" s="88" t="s">
+        <v>138</v>
+      </c>
+      <c r="D42" s="85" t="s">
+        <v>127</v>
       </c>
       <c r="E42" s="32" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="F42" s="36">
         <v>45078</v>
@@ -2998,13 +2974,13 @@
     <row r="43" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A43" s="9"/>
       <c r="B43" s="43" t="s">
-        <v>133</v>
-      </c>
-      <c r="C43" s="108" t="s">
-        <v>159</v>
-      </c>
-      <c r="D43" s="102" t="s">
-        <v>148</v>
+        <v>113</v>
+      </c>
+      <c r="C43" s="87" t="s">
+        <v>139</v>
+      </c>
+      <c r="D43" s="81" t="s">
+        <v>128</v>
       </c>
       <c r="E43" s="29" t="s">
         <v>48</v>
@@ -3025,13 +3001,13 @@
     <row r="44" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A44" s="9"/>
       <c r="B44" s="43" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="C44" s="44" t="s">
-        <v>160</v>
-      </c>
-      <c r="D44" s="102" t="s">
-        <v>149</v>
+        <v>140</v>
+      </c>
+      <c r="D44" s="81" t="s">
+        <v>129</v>
       </c>
       <c r="E44" s="32" t="s">
         <v>30</v>
@@ -3052,13 +3028,13 @@
     <row r="45" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A45" s="9"/>
       <c r="B45" s="57" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="C45" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="D45" s="102" t="s">
-        <v>150</v>
+        <v>141</v>
+      </c>
+      <c r="D45" s="81" t="s">
+        <v>130</v>
       </c>
       <c r="E45" s="32" t="s">
         <v>30</v>
@@ -3082,10 +3058,10 @@
         <v>82</v>
       </c>
       <c r="C46" s="44" t="s">
-        <v>178</v>
-      </c>
-      <c r="D46" s="98" t="s">
-        <v>151</v>
+        <v>158</v>
+      </c>
+      <c r="D46" s="77" t="s">
+        <v>131</v>
       </c>
       <c r="E46" s="32" t="s">
         <v>33</v>
@@ -3109,10 +3085,10 @@
         <v>83</v>
       </c>
       <c r="C47" s="47" t="s">
-        <v>168</v>
-      </c>
-      <c r="D47" s="101" t="s">
-        <v>184</v>
+        <v>148</v>
+      </c>
+      <c r="D47" s="80" t="s">
+        <v>164</v>
       </c>
       <c r="E47" s="48" t="s">
         <v>61</v>
@@ -3138,8 +3114,8 @@
       <c r="C48" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="D48" s="98" t="s">
-        <v>139</v>
+      <c r="D48" s="77" t="s">
+        <v>119</v>
       </c>
       <c r="E48" s="48" t="s">
         <v>61</v>
@@ -3163,10 +3139,10 @@
         <v>84</v>
       </c>
       <c r="C49" s="47" t="s">
-        <v>179</v>
-      </c>
-      <c r="D49" s="98" t="s">
-        <v>180</v>
+        <v>159</v>
+      </c>
+      <c r="D49" s="77" t="s">
+        <v>160</v>
       </c>
       <c r="E49" s="48" t="s">
         <v>48</v>
@@ -3194,8 +3170,8 @@
       <c r="C50" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="D50" s="102" t="s">
-        <v>183</v>
+      <c r="D50" s="81" t="s">
+        <v>163</v>
       </c>
       <c r="E50" s="48" t="s">
         <v>65</v>
@@ -3221,8 +3197,8 @@
       <c r="C51" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="D51" s="98" t="s">
-        <v>152</v>
+      <c r="D51" s="77" t="s">
+        <v>132</v>
       </c>
       <c r="E51" s="48" t="s">
         <v>65</v>
@@ -3250,8 +3226,8 @@
       <c r="C52" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="D52" s="98" t="s">
-        <v>153</v>
+      <c r="D52" s="77" t="s">
+        <v>133</v>
       </c>
       <c r="E52" s="48" t="s">
         <v>48</v>
@@ -3277,7 +3253,7 @@
         <v>91</v>
       </c>
       <c r="C53" s="61"/>
-      <c r="D53" s="103"/>
+      <c r="D53" s="82"/>
       <c r="E53" s="62"/>
       <c r="F53" s="63">
         <f>F40</f>
@@ -5054,7 +5030,7 @@
     <mergeCell ref="I26:I27"/>
     <mergeCell ref="I28:I30"/>
   </mergeCells>
-  <phoneticPr fontId="50" type="noConversion"/>
+  <phoneticPr fontId="41" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D37" r:id="rId1" display="http://sgds.rds-02.py/" xr:uid="{36ADFF1F-D13D-4674-B357-8868DDDCF9E7}"/>
     <hyperlink ref="D40" r:id="rId2" display="http://04.py/" xr:uid="{7E6EEFD5-183D-4445-942A-8164C7007BC5}"/>
@@ -5071,19 +5047,544 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50EA98F-4DD8-4D92-86C4-FE2038E01CE5}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:H26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="62.42578125" customWidth="1"/>
+    <col min="3" max="3" width="52.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="81.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="23.25">
+      <c r="A1" s="112" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1"/>
+      <c r="B2" s="113" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="114"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1"/>
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1"/>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1"/>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1"/>
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="8">
+        <v>45107</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1"/>
+      <c r="B7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="8">
+        <v>45112</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" spans="1:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="76" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" thickBot="1">
+      <c r="A10" s="9"/>
+      <c r="B10" s="90" t="s">
+        <v>166</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="D10" s="104" t="s">
+        <v>182</v>
+      </c>
+      <c r="E10" s="95" t="s">
+        <v>173</v>
+      </c>
+      <c r="F10" s="99">
+        <f>C6</f>
+        <v>45107</v>
+      </c>
+      <c r="G10" s="99">
+        <v>45107</v>
+      </c>
+      <c r="H10" s="103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" thickBot="1">
+      <c r="A11" s="9"/>
+      <c r="B11" s="89" t="s">
+        <v>167</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="104" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" s="95" t="s">
+        <v>173</v>
+      </c>
+      <c r="F11" s="99">
+        <v>45107</v>
+      </c>
+      <c r="G11" s="98">
+        <v>45108</v>
+      </c>
+      <c r="H11" s="103">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" thickBot="1">
+      <c r="A12" s="9"/>
+      <c r="B12" s="89" t="s">
+        <v>171</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="104" t="s">
+        <v>156</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="99">
+        <v>45108</v>
+      </c>
+      <c r="G12" s="100">
+        <v>45108</v>
+      </c>
+      <c r="H12" s="103"/>
+    </row>
+    <row r="13" spans="1:8" ht="15" thickBot="1">
+      <c r="A13" s="9"/>
+      <c r="B13" s="89" t="s">
+        <v>168</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="104" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="95" t="s">
+        <v>173</v>
+      </c>
+      <c r="F13" s="99">
+        <v>45108</v>
+      </c>
+      <c r="G13" s="100">
+        <v>45108</v>
+      </c>
+      <c r="H13" s="103"/>
+    </row>
+    <row r="14" spans="1:8" ht="15" thickBot="1">
+      <c r="A14" s="9"/>
+      <c r="B14" s="89" t="s">
+        <v>170</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="104" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" s="96" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="99">
+        <v>45108</v>
+      </c>
+      <c r="G14" s="100">
+        <v>45108</v>
+      </c>
+      <c r="H14" s="103"/>
+    </row>
+    <row r="15" spans="1:8" ht="15" thickBot="1">
+      <c r="A15" s="9"/>
+      <c r="B15" s="89" t="s">
+        <v>172</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="104" t="s">
+        <v>119</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="99">
+        <v>45108</v>
+      </c>
+      <c r="G15" s="100">
+        <v>45108</v>
+      </c>
+      <c r="H15" s="103"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A16" s="9"/>
+      <c r="B16" s="89" t="s">
+        <v>169</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="104" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="99">
+        <v>45108</v>
+      </c>
+      <c r="G16" s="100">
+        <v>45108</v>
+      </c>
+      <c r="H16" s="103"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A17" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="39"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="41">
+        <v>45107</v>
+      </c>
+      <c r="G17" s="41">
+        <v>45108</v>
+      </c>
+      <c r="H17" s="42">
+        <f>SUM(H10:H16)/7</f>
+        <v>0.25714285714285717</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15" thickBot="1">
+      <c r="A18" s="9"/>
+      <c r="B18" s="91" t="s">
+        <v>177</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="D18" s="107" t="s">
+        <v>131</v>
+      </c>
+      <c r="E18" s="96" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="101">
+        <v>45109</v>
+      </c>
+      <c r="G18" s="101">
+        <v>45109</v>
+      </c>
+      <c r="H18" s="102"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" thickBot="1">
+      <c r="A19" s="9"/>
+      <c r="B19" s="91" t="s">
+        <v>174</v>
+      </c>
+      <c r="C19" s="94"/>
+      <c r="D19" s="105"/>
+      <c r="E19" s="95"/>
+      <c r="F19" s="101">
+        <v>45109</v>
+      </c>
+      <c r="G19" s="101">
+        <v>45109</v>
+      </c>
+      <c r="H19" s="102"/>
+    </row>
+    <row r="20" spans="1:8" ht="15" thickBot="1">
+      <c r="A20" s="9"/>
+      <c r="B20" s="91" t="s">
+        <v>175</v>
+      </c>
+      <c r="C20" s="94"/>
+      <c r="D20" s="105"/>
+      <c r="E20" s="95"/>
+      <c r="F20" s="101">
+        <v>45109</v>
+      </c>
+      <c r="G20" s="101">
+        <v>45109</v>
+      </c>
+      <c r="H20" s="102"/>
+    </row>
+    <row r="21" spans="1:8" ht="15" thickBot="1">
+      <c r="A21" s="9"/>
+      <c r="B21" s="91" t="s">
+        <v>176</v>
+      </c>
+      <c r="C21" s="94"/>
+      <c r="D21" s="106"/>
+      <c r="E21" s="96"/>
+      <c r="F21" s="101">
+        <v>45109</v>
+      </c>
+      <c r="G21" s="101">
+        <v>45110</v>
+      </c>
+      <c r="H21" s="102"/>
+    </row>
+    <row r="22" spans="1:8" ht="15" thickBot="1">
+      <c r="A22" s="9"/>
+      <c r="B22" s="91" t="s">
+        <v>178</v>
+      </c>
+      <c r="C22" s="47" t="s">
+        <v>148</v>
+      </c>
+      <c r="D22" s="108" t="s">
+        <v>164</v>
+      </c>
+      <c r="E22" s="97" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" s="101">
+        <v>45109</v>
+      </c>
+      <c r="G22" s="101">
+        <v>45111</v>
+      </c>
+      <c r="H22" s="102"/>
+    </row>
+    <row r="23" spans="1:8" ht="15" thickBot="1">
+      <c r="A23" s="9"/>
+      <c r="B23" s="89" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="47" t="s">
+        <v>159</v>
+      </c>
+      <c r="D23" s="107" t="s">
+        <v>180</v>
+      </c>
+      <c r="E23" s="97" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" s="101">
+        <v>45111</v>
+      </c>
+      <c r="G23" s="101">
+        <v>45111</v>
+      </c>
+      <c r="H23" s="102"/>
+    </row>
+    <row r="24" spans="1:8" ht="15" thickBot="1">
+      <c r="A24" s="9"/>
+      <c r="B24" s="92" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="109" t="s">
+        <v>162</v>
+      </c>
+      <c r="E24" s="97" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" s="101">
+        <v>45111</v>
+      </c>
+      <c r="G24" s="101">
+        <v>45111</v>
+      </c>
+      <c r="H24" s="102"/>
+    </row>
+    <row r="25" spans="1:8" ht="15" thickBot="1">
+      <c r="A25" s="9"/>
+      <c r="B25" s="93" t="s">
+        <v>179</v>
+      </c>
+      <c r="C25" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="D25" s="107" t="s">
+        <v>184</v>
+      </c>
+      <c r="E25" s="95" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="101">
+        <v>45112</v>
+      </c>
+      <c r="G25" s="101">
+        <v>45112</v>
+      </c>
+      <c r="H25" s="102"/>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A26" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="86"/>
+      <c r="D26" s="78"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="55">
+        <v>45109</v>
+      </c>
+      <c r="G26" s="41">
+        <v>45112</v>
+      </c>
+      <c r="H26" s="56">
+        <f>SUM(H18:H25)/8</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D24" r:id="rId1" display="http://sgds.rds-02.py/" xr:uid="{9B119A75-9F9D-420B-A8DA-DC877DBFE7BA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="B1:C1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="31.42578125" customWidth="1"/>
-    <col min="3" max="3" width="47.140625" customWidth="1"/>
+    <col min="3" max="3" width="50.140625" customWidth="1"/>
     <col min="4" max="6" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6160,1176 +6661,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="B1:M1000"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
-  <cols>
-    <col min="1" max="6" width="12.5703125" customWidth="1"/>
-    <col min="8" max="8" width="6" customWidth="1"/>
-    <col min="9" max="9" width="30.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:13" ht="15.75" customHeight="1"/>
-    <row r="2" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B2" s="76" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="2:13" ht="15.75" customHeight="1">
-      <c r="J3" s="77" t="s">
-        <v>109</v>
-      </c>
-      <c r="K3" s="78" t="s">
-        <v>110</v>
-      </c>
-      <c r="L3" s="79" t="s">
-        <v>111</v>
-      </c>
-      <c r="M3" s="80" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B4" s="81" t="s">
-        <v>113</v>
-      </c>
-      <c r="F4" s="81" t="s">
-        <v>114</v>
-      </c>
-      <c r="G4" s="82" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" s="83">
-        <v>1</v>
-      </c>
-      <c r="I4" s="84" t="s">
-        <v>115</v>
-      </c>
-      <c r="K4" s="85" t="s">
-        <v>116</v>
-      </c>
-      <c r="L4" s="81" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" ht="15.75" customHeight="1">
-      <c r="G5" s="82" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" s="83">
-        <f t="shared" ref="H5:H13" si="0">H4+1</f>
-        <v>2</v>
-      </c>
-      <c r="I5" s="84" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" ht="15.75" customHeight="1">
-      <c r="G6" s="82" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="86">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I6" s="87" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" ht="15.75" customHeight="1">
-      <c r="G7" s="82" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" s="86">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="I7" s="87" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" ht="15.75" customHeight="1">
-      <c r="G8" s="82" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" s="88">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="I8" s="89" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" ht="15.75" customHeight="1">
-      <c r="G9" s="82" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" s="88">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="I9" s="89" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" ht="15.75" customHeight="1">
-      <c r="G10" s="82" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10" s="90">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="I10" s="91" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" ht="15.75" customHeight="1">
-      <c r="G11" s="82" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" s="83">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="I11" s="84" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" ht="15.75" customHeight="1">
-      <c r="G12" s="82" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" s="92">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="I12" s="93" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13" ht="15.75" customHeight="1">
-      <c r="G13" s="82" t="b">
-        <v>0</v>
-      </c>
-      <c r="H13" s="92">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I13" s="94" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" ht="15.75" customHeight="1">
-      <c r="G14" s="82" t="b">
-        <v>0</v>
-      </c>
-      <c r="H14" s="95">
-        <v>11</v>
-      </c>
-      <c r="I14" s="82" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13" ht="15.75" customHeight="1">
-      <c r="H15" s="96"/>
-    </row>
-    <row r="16" spans="2:13" ht="15.75" customHeight="1"/>
-    <row r="17" ht="15.75" customHeight="1"/>
-    <row r="18" ht="15.75" customHeight="1"/>
-    <row r="19" ht="15.75" customHeight="1"/>
-    <row r="20" ht="15.75" customHeight="1"/>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
-    <row r="37" ht="15.75" customHeight="1"/>
-    <row r="38" ht="15.75" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
-    <row r="65" ht="15.75" customHeight="1"/>
-    <row r="66" ht="15.75" customHeight="1"/>
-    <row r="67" ht="15.75" customHeight="1"/>
-    <row r="68" ht="15.75" customHeight="1"/>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
-    <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1"/>
-    <row r="73" ht="15.75" customHeight="1"/>
-    <row r="74" ht="15.75" customHeight="1"/>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="78" ht="15.75" customHeight="1"/>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
-    <row r="81" ht="15.75" customHeight="1"/>
-    <row r="82" ht="15.75" customHeight="1"/>
-    <row r="83" ht="15.75" customHeight="1"/>
-    <row r="84" ht="15.75" customHeight="1"/>
-    <row r="85" ht="15.75" customHeight="1"/>
-    <row r="86" ht="15.75" customHeight="1"/>
-    <row r="87" ht="15.75" customHeight="1"/>
-    <row r="88" ht="15.75" customHeight="1"/>
-    <row r="89" ht="15.75" customHeight="1"/>
-    <row r="90" ht="15.75" customHeight="1"/>
-    <row r="91" ht="15.75" customHeight="1"/>
-    <row r="92" ht="15.75" customHeight="1"/>
-    <row r="93" ht="15.75" customHeight="1"/>
-    <row r="94" ht="15.75" customHeight="1"/>
-    <row r="95" ht="15.75" customHeight="1"/>
-    <row r="96" ht="15.75" customHeight="1"/>
-    <row r="97" ht="15.75" customHeight="1"/>
-    <row r="98" ht="15.75" customHeight="1"/>
-    <row r="99" ht="15.75" customHeight="1"/>
-    <row r="100" ht="15.75" customHeight="1"/>
-    <row r="101" ht="15.75" customHeight="1"/>
-    <row r="102" ht="15.75" customHeight="1"/>
-    <row r="103" ht="15.75" customHeight="1"/>
-    <row r="104" ht="15.75" customHeight="1"/>
-    <row r="105" ht="15.75" customHeight="1"/>
-    <row r="106" ht="15.75" customHeight="1"/>
-    <row r="107" ht="15.75" customHeight="1"/>
-    <row r="108" ht="15.75" customHeight="1"/>
-    <row r="109" ht="15.75" customHeight="1"/>
-    <row r="110" ht="15.75" customHeight="1"/>
-    <row r="111" ht="15.75" customHeight="1"/>
-    <row r="112" ht="15.75" customHeight="1"/>
-    <row r="113" ht="15.75" customHeight="1"/>
-    <row r="114" ht="15.75" customHeight="1"/>
-    <row r="115" ht="15.75" customHeight="1"/>
-    <row r="116" ht="15.75" customHeight="1"/>
-    <row r="117" ht="15.75" customHeight="1"/>
-    <row r="118" ht="15.75" customHeight="1"/>
-    <row r="119" ht="15.75" customHeight="1"/>
-    <row r="120" ht="15.75" customHeight="1"/>
-    <row r="121" ht="15.75" customHeight="1"/>
-    <row r="122" ht="15.75" customHeight="1"/>
-    <row r="123" ht="15.75" customHeight="1"/>
-    <row r="124" ht="15.75" customHeight="1"/>
-    <row r="125" ht="15.75" customHeight="1"/>
-    <row r="126" ht="15.75" customHeight="1"/>
-    <row r="127" ht="15.75" customHeight="1"/>
-    <row r="128" ht="15.75" customHeight="1"/>
-    <row r="129" ht="15.75" customHeight="1"/>
-    <row r="130" ht="15.75" customHeight="1"/>
-    <row r="131" ht="15.75" customHeight="1"/>
-    <row r="132" ht="15.75" customHeight="1"/>
-    <row r="133" ht="15.75" customHeight="1"/>
-    <row r="134" ht="15.75" customHeight="1"/>
-    <row r="135" ht="15.75" customHeight="1"/>
-    <row r="136" ht="15.75" customHeight="1"/>
-    <row r="137" ht="15.75" customHeight="1"/>
-    <row r="138" ht="15.75" customHeight="1"/>
-    <row r="139" ht="15.75" customHeight="1"/>
-    <row r="140" ht="15.75" customHeight="1"/>
-    <row r="141" ht="15.75" customHeight="1"/>
-    <row r="142" ht="15.75" customHeight="1"/>
-    <row r="143" ht="15.75" customHeight="1"/>
-    <row r="144" ht="15.75" customHeight="1"/>
-    <row r="145" ht="15.75" customHeight="1"/>
-    <row r="146" ht="15.75" customHeight="1"/>
-    <row r="147" ht="15.75" customHeight="1"/>
-    <row r="148" ht="15.75" customHeight="1"/>
-    <row r="149" ht="15.75" customHeight="1"/>
-    <row r="150" ht="15.75" customHeight="1"/>
-    <row r="151" ht="15.75" customHeight="1"/>
-    <row r="152" ht="15.75" customHeight="1"/>
-    <row r="153" ht="15.75" customHeight="1"/>
-    <row r="154" ht="15.75" customHeight="1"/>
-    <row r="155" ht="15.75" customHeight="1"/>
-    <row r="156" ht="15.75" customHeight="1"/>
-    <row r="157" ht="15.75" customHeight="1"/>
-    <row r="158" ht="15.75" customHeight="1"/>
-    <row r="159" ht="15.75" customHeight="1"/>
-    <row r="160" ht="15.75" customHeight="1"/>
-    <row r="161" ht="15.75" customHeight="1"/>
-    <row r="162" ht="15.75" customHeight="1"/>
-    <row r="163" ht="15.75" customHeight="1"/>
-    <row r="164" ht="15.75" customHeight="1"/>
-    <row r="165" ht="15.75" customHeight="1"/>
-    <row r="166" ht="15.75" customHeight="1"/>
-    <row r="167" ht="15.75" customHeight="1"/>
-    <row r="168" ht="15.75" customHeight="1"/>
-    <row r="169" ht="15.75" customHeight="1"/>
-    <row r="170" ht="15.75" customHeight="1"/>
-    <row r="171" ht="15.75" customHeight="1"/>
-    <row r="172" ht="15.75" customHeight="1"/>
-    <row r="173" ht="15.75" customHeight="1"/>
-    <row r="174" ht="15.75" customHeight="1"/>
-    <row r="175" ht="15.75" customHeight="1"/>
-    <row r="176" ht="15.75" customHeight="1"/>
-    <row r="177" ht="15.75" customHeight="1"/>
-    <row r="178" ht="15.75" customHeight="1"/>
-    <row r="179" ht="15.75" customHeight="1"/>
-    <row r="180" ht="15.75" customHeight="1"/>
-    <row r="181" ht="15.75" customHeight="1"/>
-    <row r="182" ht="15.75" customHeight="1"/>
-    <row r="183" ht="15.75" customHeight="1"/>
-    <row r="184" ht="15.75" customHeight="1"/>
-    <row r="185" ht="15.75" customHeight="1"/>
-    <row r="186" ht="15.75" customHeight="1"/>
-    <row r="187" ht="15.75" customHeight="1"/>
-    <row r="188" ht="15.75" customHeight="1"/>
-    <row r="189" ht="15.75" customHeight="1"/>
-    <row r="190" ht="15.75" customHeight="1"/>
-    <row r="191" ht="15.75" customHeight="1"/>
-    <row r="192" ht="15.75" customHeight="1"/>
-    <row r="193" ht="15.75" customHeight="1"/>
-    <row r="194" ht="15.75" customHeight="1"/>
-    <row r="195" ht="15.75" customHeight="1"/>
-    <row r="196" ht="15.75" customHeight="1"/>
-    <row r="197" ht="15.75" customHeight="1"/>
-    <row r="198" ht="15.75" customHeight="1"/>
-    <row r="199" ht="15.75" customHeight="1"/>
-    <row r="200" ht="15.75" customHeight="1"/>
-    <row r="201" ht="15.75" customHeight="1"/>
-    <row r="202" ht="15.75" customHeight="1"/>
-    <row r="203" ht="15.75" customHeight="1"/>
-    <row r="204" ht="15.75" customHeight="1"/>
-    <row r="205" ht="15.75" customHeight="1"/>
-    <row r="206" ht="15.75" customHeight="1"/>
-    <row r="207" ht="15.75" customHeight="1"/>
-    <row r="208" ht="15.75" customHeight="1"/>
-    <row r="209" ht="15.75" customHeight="1"/>
-    <row r="210" ht="15.75" customHeight="1"/>
-    <row r="211" ht="15.75" customHeight="1"/>
-    <row r="212" ht="15.75" customHeight="1"/>
-    <row r="213" ht="15.75" customHeight="1"/>
-    <row r="214" ht="15.75" customHeight="1"/>
-    <row r="215" ht="15.75" customHeight="1"/>
-    <row r="216" ht="15.75" customHeight="1"/>
-    <row r="217" ht="15.75" customHeight="1"/>
-    <row r="218" ht="15.75" customHeight="1"/>
-    <row r="219" ht="15.75" customHeight="1"/>
-    <row r="220" ht="15.75" customHeight="1"/>
-    <row r="221" ht="15.75" customHeight="1"/>
-    <row r="222" ht="15.75" customHeight="1"/>
-    <row r="223" ht="15.75" customHeight="1"/>
-    <row r="224" ht="15.75" customHeight="1"/>
-    <row r="225" ht="15.75" customHeight="1"/>
-    <row r="226" ht="15.75" customHeight="1"/>
-    <row r="227" ht="15.75" customHeight="1"/>
-    <row r="228" ht="15.75" customHeight="1"/>
-    <row r="229" ht="15.75" customHeight="1"/>
-    <row r="230" ht="15.75" customHeight="1"/>
-    <row r="231" ht="15.75" customHeight="1"/>
-    <row r="232" ht="15.75" customHeight="1"/>
-    <row r="233" ht="15.75" customHeight="1"/>
-    <row r="234" ht="15.75" customHeight="1"/>
-    <row r="235" ht="15.75" customHeight="1"/>
-    <row r="236" ht="15.75" customHeight="1"/>
-    <row r="237" ht="15.75" customHeight="1"/>
-    <row r="238" ht="15.75" customHeight="1"/>
-    <row r="239" ht="15.75" customHeight="1"/>
-    <row r="240" ht="15.75" customHeight="1"/>
-    <row r="241" ht="15.75" customHeight="1"/>
-    <row r="242" ht="15.75" customHeight="1"/>
-    <row r="243" ht="15.75" customHeight="1"/>
-    <row r="244" ht="15.75" customHeight="1"/>
-    <row r="245" ht="15.75" customHeight="1"/>
-    <row r="246" ht="15.75" customHeight="1"/>
-    <row r="247" ht="15.75" customHeight="1"/>
-    <row r="248" ht="15.75" customHeight="1"/>
-    <row r="249" ht="15.75" customHeight="1"/>
-    <row r="250" ht="15.75" customHeight="1"/>
-    <row r="251" ht="15.75" customHeight="1"/>
-    <row r="252" ht="15.75" customHeight="1"/>
-    <row r="253" ht="15.75" customHeight="1"/>
-    <row r="254" ht="15.75" customHeight="1"/>
-    <row r="255" ht="15.75" customHeight="1"/>
-    <row r="256" ht="15.75" customHeight="1"/>
-    <row r="257" ht="15.75" customHeight="1"/>
-    <row r="258" ht="15.75" customHeight="1"/>
-    <row r="259" ht="15.75" customHeight="1"/>
-    <row r="260" ht="15.75" customHeight="1"/>
-    <row r="261" ht="15.75" customHeight="1"/>
-    <row r="262" ht="15.75" customHeight="1"/>
-    <row r="263" ht="15.75" customHeight="1"/>
-    <row r="264" ht="15.75" customHeight="1"/>
-    <row r="265" ht="15.75" customHeight="1"/>
-    <row r="266" ht="15.75" customHeight="1"/>
-    <row r="267" ht="15.75" customHeight="1"/>
-    <row r="268" ht="15.75" customHeight="1"/>
-    <row r="269" ht="15.75" customHeight="1"/>
-    <row r="270" ht="15.75" customHeight="1"/>
-    <row r="271" ht="15.75" customHeight="1"/>
-    <row r="272" ht="15.75" customHeight="1"/>
-    <row r="273" ht="15.75" customHeight="1"/>
-    <row r="274" ht="15.75" customHeight="1"/>
-    <row r="275" ht="15.75" customHeight="1"/>
-    <row r="276" ht="15.75" customHeight="1"/>
-    <row r="277" ht="15.75" customHeight="1"/>
-    <row r="278" ht="15.75" customHeight="1"/>
-    <row r="279" ht="15.75" customHeight="1"/>
-    <row r="280" ht="15.75" customHeight="1"/>
-    <row r="281" ht="15.75" customHeight="1"/>
-    <row r="282" ht="15.75" customHeight="1"/>
-    <row r="283" ht="15.75" customHeight="1"/>
-    <row r="284" ht="15.75" customHeight="1"/>
-    <row r="285" ht="15.75" customHeight="1"/>
-    <row r="286" ht="15.75" customHeight="1"/>
-    <row r="287" ht="15.75" customHeight="1"/>
-    <row r="288" ht="15.75" customHeight="1"/>
-    <row r="289" ht="15.75" customHeight="1"/>
-    <row r="290" ht="15.75" customHeight="1"/>
-    <row r="291" ht="15.75" customHeight="1"/>
-    <row r="292" ht="15.75" customHeight="1"/>
-    <row r="293" ht="15.75" customHeight="1"/>
-    <row r="294" ht="15.75" customHeight="1"/>
-    <row r="295" ht="15.75" customHeight="1"/>
-    <row r="296" ht="15.75" customHeight="1"/>
-    <row r="297" ht="15.75" customHeight="1"/>
-    <row r="298" ht="15.75" customHeight="1"/>
-    <row r="299" ht="15.75" customHeight="1"/>
-    <row r="300" ht="15.75" customHeight="1"/>
-    <row r="301" ht="15.75" customHeight="1"/>
-    <row r="302" ht="15.75" customHeight="1"/>
-    <row r="303" ht="15.75" customHeight="1"/>
-    <row r="304" ht="15.75" customHeight="1"/>
-    <row r="305" ht="15.75" customHeight="1"/>
-    <row r="306" ht="15.75" customHeight="1"/>
-    <row r="307" ht="15.75" customHeight="1"/>
-    <row r="308" ht="15.75" customHeight="1"/>
-    <row r="309" ht="15.75" customHeight="1"/>
-    <row r="310" ht="15.75" customHeight="1"/>
-    <row r="311" ht="15.75" customHeight="1"/>
-    <row r="312" ht="15.75" customHeight="1"/>
-    <row r="313" ht="15.75" customHeight="1"/>
-    <row r="314" ht="15.75" customHeight="1"/>
-    <row r="315" ht="15.75" customHeight="1"/>
-    <row r="316" ht="15.75" customHeight="1"/>
-    <row r="317" ht="15.75" customHeight="1"/>
-    <row r="318" ht="15.75" customHeight="1"/>
-    <row r="319" ht="15.75" customHeight="1"/>
-    <row r="320" ht="15.75" customHeight="1"/>
-    <row r="321" ht="15.75" customHeight="1"/>
-    <row r="322" ht="15.75" customHeight="1"/>
-    <row r="323" ht="15.75" customHeight="1"/>
-    <row r="324" ht="15.75" customHeight="1"/>
-    <row r="325" ht="15.75" customHeight="1"/>
-    <row r="326" ht="15.75" customHeight="1"/>
-    <row r="327" ht="15.75" customHeight="1"/>
-    <row r="328" ht="15.75" customHeight="1"/>
-    <row r="329" ht="15.75" customHeight="1"/>
-    <row r="330" ht="15.75" customHeight="1"/>
-    <row r="331" ht="15.75" customHeight="1"/>
-    <row r="332" ht="15.75" customHeight="1"/>
-    <row r="333" ht="15.75" customHeight="1"/>
-    <row r="334" ht="15.75" customHeight="1"/>
-    <row r="335" ht="15.75" customHeight="1"/>
-    <row r="336" ht="15.75" customHeight="1"/>
-    <row r="337" ht="15.75" customHeight="1"/>
-    <row r="338" ht="15.75" customHeight="1"/>
-    <row r="339" ht="15.75" customHeight="1"/>
-    <row r="340" ht="15.75" customHeight="1"/>
-    <row r="341" ht="15.75" customHeight="1"/>
-    <row r="342" ht="15.75" customHeight="1"/>
-    <row r="343" ht="15.75" customHeight="1"/>
-    <row r="344" ht="15.75" customHeight="1"/>
-    <row r="345" ht="15.75" customHeight="1"/>
-    <row r="346" ht="15.75" customHeight="1"/>
-    <row r="347" ht="15.75" customHeight="1"/>
-    <row r="348" ht="15.75" customHeight="1"/>
-    <row r="349" ht="15.75" customHeight="1"/>
-    <row r="350" ht="15.75" customHeight="1"/>
-    <row r="351" ht="15.75" customHeight="1"/>
-    <row r="352" ht="15.75" customHeight="1"/>
-    <row r="353" ht="15.75" customHeight="1"/>
-    <row r="354" ht="15.75" customHeight="1"/>
-    <row r="355" ht="15.75" customHeight="1"/>
-    <row r="356" ht="15.75" customHeight="1"/>
-    <row r="357" ht="15.75" customHeight="1"/>
-    <row r="358" ht="15.75" customHeight="1"/>
-    <row r="359" ht="15.75" customHeight="1"/>
-    <row r="360" ht="15.75" customHeight="1"/>
-    <row r="361" ht="15.75" customHeight="1"/>
-    <row r="362" ht="15.75" customHeight="1"/>
-    <row r="363" ht="15.75" customHeight="1"/>
-    <row r="364" ht="15.75" customHeight="1"/>
-    <row r="365" ht="15.75" customHeight="1"/>
-    <row r="366" ht="15.75" customHeight="1"/>
-    <row r="367" ht="15.75" customHeight="1"/>
-    <row r="368" ht="15.75" customHeight="1"/>
-    <row r="369" ht="15.75" customHeight="1"/>
-    <row r="370" ht="15.75" customHeight="1"/>
-    <row r="371" ht="15.75" customHeight="1"/>
-    <row r="372" ht="15.75" customHeight="1"/>
-    <row r="373" ht="15.75" customHeight="1"/>
-    <row r="374" ht="15.75" customHeight="1"/>
-    <row r="375" ht="15.75" customHeight="1"/>
-    <row r="376" ht="15.75" customHeight="1"/>
-    <row r="377" ht="15.75" customHeight="1"/>
-    <row r="378" ht="15.75" customHeight="1"/>
-    <row r="379" ht="15.75" customHeight="1"/>
-    <row r="380" ht="15.75" customHeight="1"/>
-    <row r="381" ht="15.75" customHeight="1"/>
-    <row r="382" ht="15.75" customHeight="1"/>
-    <row r="383" ht="15.75" customHeight="1"/>
-    <row r="384" ht="15.75" customHeight="1"/>
-    <row r="385" ht="15.75" customHeight="1"/>
-    <row r="386" ht="15.75" customHeight="1"/>
-    <row r="387" ht="15.75" customHeight="1"/>
-    <row r="388" ht="15.75" customHeight="1"/>
-    <row r="389" ht="15.75" customHeight="1"/>
-    <row r="390" ht="15.75" customHeight="1"/>
-    <row r="391" ht="15.75" customHeight="1"/>
-    <row r="392" ht="15.75" customHeight="1"/>
-    <row r="393" ht="15.75" customHeight="1"/>
-    <row r="394" ht="15.75" customHeight="1"/>
-    <row r="395" ht="15.75" customHeight="1"/>
-    <row r="396" ht="15.75" customHeight="1"/>
-    <row r="397" ht="15.75" customHeight="1"/>
-    <row r="398" ht="15.75" customHeight="1"/>
-    <row r="399" ht="15.75" customHeight="1"/>
-    <row r="400" ht="15.75" customHeight="1"/>
-    <row r="401" ht="15.75" customHeight="1"/>
-    <row r="402" ht="15.75" customHeight="1"/>
-    <row r="403" ht="15.75" customHeight="1"/>
-    <row r="404" ht="15.75" customHeight="1"/>
-    <row r="405" ht="15.75" customHeight="1"/>
-    <row r="406" ht="15.75" customHeight="1"/>
-    <row r="407" ht="15.75" customHeight="1"/>
-    <row r="408" ht="15.75" customHeight="1"/>
-    <row r="409" ht="15.75" customHeight="1"/>
-    <row r="410" ht="15.75" customHeight="1"/>
-    <row r="411" ht="15.75" customHeight="1"/>
-    <row r="412" ht="15.75" customHeight="1"/>
-    <row r="413" ht="15.75" customHeight="1"/>
-    <row r="414" ht="15.75" customHeight="1"/>
-    <row r="415" ht="15.75" customHeight="1"/>
-    <row r="416" ht="15.75" customHeight="1"/>
-    <row r="417" ht="15.75" customHeight="1"/>
-    <row r="418" ht="15.75" customHeight="1"/>
-    <row r="419" ht="15.75" customHeight="1"/>
-    <row r="420" ht="15.75" customHeight="1"/>
-    <row r="421" ht="15.75" customHeight="1"/>
-    <row r="422" ht="15.75" customHeight="1"/>
-    <row r="423" ht="15.75" customHeight="1"/>
-    <row r="424" ht="15.75" customHeight="1"/>
-    <row r="425" ht="15.75" customHeight="1"/>
-    <row r="426" ht="15.75" customHeight="1"/>
-    <row r="427" ht="15.75" customHeight="1"/>
-    <row r="428" ht="15.75" customHeight="1"/>
-    <row r="429" ht="15.75" customHeight="1"/>
-    <row r="430" ht="15.75" customHeight="1"/>
-    <row r="431" ht="15.75" customHeight="1"/>
-    <row r="432" ht="15.75" customHeight="1"/>
-    <row r="433" ht="15.75" customHeight="1"/>
-    <row r="434" ht="15.75" customHeight="1"/>
-    <row r="435" ht="15.75" customHeight="1"/>
-    <row r="436" ht="15.75" customHeight="1"/>
-    <row r="437" ht="15.75" customHeight="1"/>
-    <row r="438" ht="15.75" customHeight="1"/>
-    <row r="439" ht="15.75" customHeight="1"/>
-    <row r="440" ht="15.75" customHeight="1"/>
-    <row r="441" ht="15.75" customHeight="1"/>
-    <row r="442" ht="15.75" customHeight="1"/>
-    <row r="443" ht="15.75" customHeight="1"/>
-    <row r="444" ht="15.75" customHeight="1"/>
-    <row r="445" ht="15.75" customHeight="1"/>
-    <row r="446" ht="15.75" customHeight="1"/>
-    <row r="447" ht="15.75" customHeight="1"/>
-    <row r="448" ht="15.75" customHeight="1"/>
-    <row r="449" ht="15.75" customHeight="1"/>
-    <row r="450" ht="15.75" customHeight="1"/>
-    <row r="451" ht="15.75" customHeight="1"/>
-    <row r="452" ht="15.75" customHeight="1"/>
-    <row r="453" ht="15.75" customHeight="1"/>
-    <row r="454" ht="15.75" customHeight="1"/>
-    <row r="455" ht="15.75" customHeight="1"/>
-    <row r="456" ht="15.75" customHeight="1"/>
-    <row r="457" ht="15.75" customHeight="1"/>
-    <row r="458" ht="15.75" customHeight="1"/>
-    <row r="459" ht="15.75" customHeight="1"/>
-    <row r="460" ht="15.75" customHeight="1"/>
-    <row r="461" ht="15.75" customHeight="1"/>
-    <row r="462" ht="15.75" customHeight="1"/>
-    <row r="463" ht="15.75" customHeight="1"/>
-    <row r="464" ht="15.75" customHeight="1"/>
-    <row r="465" ht="15.75" customHeight="1"/>
-    <row r="466" ht="15.75" customHeight="1"/>
-    <row r="467" ht="15.75" customHeight="1"/>
-    <row r="468" ht="15.75" customHeight="1"/>
-    <row r="469" ht="15.75" customHeight="1"/>
-    <row r="470" ht="15.75" customHeight="1"/>
-    <row r="471" ht="15.75" customHeight="1"/>
-    <row r="472" ht="15.75" customHeight="1"/>
-    <row r="473" ht="15.75" customHeight="1"/>
-    <row r="474" ht="15.75" customHeight="1"/>
-    <row r="475" ht="15.75" customHeight="1"/>
-    <row r="476" ht="15.75" customHeight="1"/>
-    <row r="477" ht="15.75" customHeight="1"/>
-    <row r="478" ht="15.75" customHeight="1"/>
-    <row r="479" ht="15.75" customHeight="1"/>
-    <row r="480" ht="15.75" customHeight="1"/>
-    <row r="481" ht="15.75" customHeight="1"/>
-    <row r="482" ht="15.75" customHeight="1"/>
-    <row r="483" ht="15.75" customHeight="1"/>
-    <row r="484" ht="15.75" customHeight="1"/>
-    <row r="485" ht="15.75" customHeight="1"/>
-    <row r="486" ht="15.75" customHeight="1"/>
-    <row r="487" ht="15.75" customHeight="1"/>
-    <row r="488" ht="15.75" customHeight="1"/>
-    <row r="489" ht="15.75" customHeight="1"/>
-    <row r="490" ht="15.75" customHeight="1"/>
-    <row r="491" ht="15.75" customHeight="1"/>
-    <row r="492" ht="15.75" customHeight="1"/>
-    <row r="493" ht="15.75" customHeight="1"/>
-    <row r="494" ht="15.75" customHeight="1"/>
-    <row r="495" ht="15.75" customHeight="1"/>
-    <row r="496" ht="15.75" customHeight="1"/>
-    <row r="497" ht="15.75" customHeight="1"/>
-    <row r="498" ht="15.75" customHeight="1"/>
-    <row r="499" ht="15.75" customHeight="1"/>
-    <row r="500" ht="15.75" customHeight="1"/>
-    <row r="501" ht="15.75" customHeight="1"/>
-    <row r="502" ht="15.75" customHeight="1"/>
-    <row r="503" ht="15.75" customHeight="1"/>
-    <row r="504" ht="15.75" customHeight="1"/>
-    <row r="505" ht="15.75" customHeight="1"/>
-    <row r="506" ht="15.75" customHeight="1"/>
-    <row r="507" ht="15.75" customHeight="1"/>
-    <row r="508" ht="15.75" customHeight="1"/>
-    <row r="509" ht="15.75" customHeight="1"/>
-    <row r="510" ht="15.75" customHeight="1"/>
-    <row r="511" ht="15.75" customHeight="1"/>
-    <row r="512" ht="15.75" customHeight="1"/>
-    <row r="513" ht="15.75" customHeight="1"/>
-    <row r="514" ht="15.75" customHeight="1"/>
-    <row r="515" ht="15.75" customHeight="1"/>
-    <row r="516" ht="15.75" customHeight="1"/>
-    <row r="517" ht="15.75" customHeight="1"/>
-    <row r="518" ht="15.75" customHeight="1"/>
-    <row r="519" ht="15.75" customHeight="1"/>
-    <row r="520" ht="15.75" customHeight="1"/>
-    <row r="521" ht="15.75" customHeight="1"/>
-    <row r="522" ht="15.75" customHeight="1"/>
-    <row r="523" ht="15.75" customHeight="1"/>
-    <row r="524" ht="15.75" customHeight="1"/>
-    <row r="525" ht="15.75" customHeight="1"/>
-    <row r="526" ht="15.75" customHeight="1"/>
-    <row r="527" ht="15.75" customHeight="1"/>
-    <row r="528" ht="15.75" customHeight="1"/>
-    <row r="529" ht="15.75" customHeight="1"/>
-    <row r="530" ht="15.75" customHeight="1"/>
-    <row r="531" ht="15.75" customHeight="1"/>
-    <row r="532" ht="15.75" customHeight="1"/>
-    <row r="533" ht="15.75" customHeight="1"/>
-    <row r="534" ht="15.75" customHeight="1"/>
-    <row r="535" ht="15.75" customHeight="1"/>
-    <row r="536" ht="15.75" customHeight="1"/>
-    <row r="537" ht="15.75" customHeight="1"/>
-    <row r="538" ht="15.75" customHeight="1"/>
-    <row r="539" ht="15.75" customHeight="1"/>
-    <row r="540" ht="15.75" customHeight="1"/>
-    <row r="541" ht="15.75" customHeight="1"/>
-    <row r="542" ht="15.75" customHeight="1"/>
-    <row r="543" ht="15.75" customHeight="1"/>
-    <row r="544" ht="15.75" customHeight="1"/>
-    <row r="545" ht="15.75" customHeight="1"/>
-    <row r="546" ht="15.75" customHeight="1"/>
-    <row r="547" ht="15.75" customHeight="1"/>
-    <row r="548" ht="15.75" customHeight="1"/>
-    <row r="549" ht="15.75" customHeight="1"/>
-    <row r="550" ht="15.75" customHeight="1"/>
-    <row r="551" ht="15.75" customHeight="1"/>
-    <row r="552" ht="15.75" customHeight="1"/>
-    <row r="553" ht="15.75" customHeight="1"/>
-    <row r="554" ht="15.75" customHeight="1"/>
-    <row r="555" ht="15.75" customHeight="1"/>
-    <row r="556" ht="15.75" customHeight="1"/>
-    <row r="557" ht="15.75" customHeight="1"/>
-    <row r="558" ht="15.75" customHeight="1"/>
-    <row r="559" ht="15.75" customHeight="1"/>
-    <row r="560" ht="15.75" customHeight="1"/>
-    <row r="561" ht="15.75" customHeight="1"/>
-    <row r="562" ht="15.75" customHeight="1"/>
-    <row r="563" ht="15.75" customHeight="1"/>
-    <row r="564" ht="15.75" customHeight="1"/>
-    <row r="565" ht="15.75" customHeight="1"/>
-    <row r="566" ht="15.75" customHeight="1"/>
-    <row r="567" ht="15.75" customHeight="1"/>
-    <row r="568" ht="15.75" customHeight="1"/>
-    <row r="569" ht="15.75" customHeight="1"/>
-    <row r="570" ht="15.75" customHeight="1"/>
-    <row r="571" ht="15.75" customHeight="1"/>
-    <row r="572" ht="15.75" customHeight="1"/>
-    <row r="573" ht="15.75" customHeight="1"/>
-    <row r="574" ht="15.75" customHeight="1"/>
-    <row r="575" ht="15.75" customHeight="1"/>
-    <row r="576" ht="15.75" customHeight="1"/>
-    <row r="577" ht="15.75" customHeight="1"/>
-    <row r="578" ht="15.75" customHeight="1"/>
-    <row r="579" ht="15.75" customHeight="1"/>
-    <row r="580" ht="15.75" customHeight="1"/>
-    <row r="581" ht="15.75" customHeight="1"/>
-    <row r="582" ht="15.75" customHeight="1"/>
-    <row r="583" ht="15.75" customHeight="1"/>
-    <row r="584" ht="15.75" customHeight="1"/>
-    <row r="585" ht="15.75" customHeight="1"/>
-    <row r="586" ht="15.75" customHeight="1"/>
-    <row r="587" ht="15.75" customHeight="1"/>
-    <row r="588" ht="15.75" customHeight="1"/>
-    <row r="589" ht="15.75" customHeight="1"/>
-    <row r="590" ht="15.75" customHeight="1"/>
-    <row r="591" ht="15.75" customHeight="1"/>
-    <row r="592" ht="15.75" customHeight="1"/>
-    <row r="593" ht="15.75" customHeight="1"/>
-    <row r="594" ht="15.75" customHeight="1"/>
-    <row r="595" ht="15.75" customHeight="1"/>
-    <row r="596" ht="15.75" customHeight="1"/>
-    <row r="597" ht="15.75" customHeight="1"/>
-    <row r="598" ht="15.75" customHeight="1"/>
-    <row r="599" ht="15.75" customHeight="1"/>
-    <row r="600" ht="15.75" customHeight="1"/>
-    <row r="601" ht="15.75" customHeight="1"/>
-    <row r="602" ht="15.75" customHeight="1"/>
-    <row r="603" ht="15.75" customHeight="1"/>
-    <row r="604" ht="15.75" customHeight="1"/>
-    <row r="605" ht="15.75" customHeight="1"/>
-    <row r="606" ht="15.75" customHeight="1"/>
-    <row r="607" ht="15.75" customHeight="1"/>
-    <row r="608" ht="15.75" customHeight="1"/>
-    <row r="609" ht="15.75" customHeight="1"/>
-    <row r="610" ht="15.75" customHeight="1"/>
-    <row r="611" ht="15.75" customHeight="1"/>
-    <row r="612" ht="15.75" customHeight="1"/>
-    <row r="613" ht="15.75" customHeight="1"/>
-    <row r="614" ht="15.75" customHeight="1"/>
-    <row r="615" ht="15.75" customHeight="1"/>
-    <row r="616" ht="15.75" customHeight="1"/>
-    <row r="617" ht="15.75" customHeight="1"/>
-    <row r="618" ht="15.75" customHeight="1"/>
-    <row r="619" ht="15.75" customHeight="1"/>
-    <row r="620" ht="15.75" customHeight="1"/>
-    <row r="621" ht="15.75" customHeight="1"/>
-    <row r="622" ht="15.75" customHeight="1"/>
-    <row r="623" ht="15.75" customHeight="1"/>
-    <row r="624" ht="15.75" customHeight="1"/>
-    <row r="625" ht="15.75" customHeight="1"/>
-    <row r="626" ht="15.75" customHeight="1"/>
-    <row r="627" ht="15.75" customHeight="1"/>
-    <row r="628" ht="15.75" customHeight="1"/>
-    <row r="629" ht="15.75" customHeight="1"/>
-    <row r="630" ht="15.75" customHeight="1"/>
-    <row r="631" ht="15.75" customHeight="1"/>
-    <row r="632" ht="15.75" customHeight="1"/>
-    <row r="633" ht="15.75" customHeight="1"/>
-    <row r="634" ht="15.75" customHeight="1"/>
-    <row r="635" ht="15.75" customHeight="1"/>
-    <row r="636" ht="15.75" customHeight="1"/>
-    <row r="637" ht="15.75" customHeight="1"/>
-    <row r="638" ht="15.75" customHeight="1"/>
-    <row r="639" ht="15.75" customHeight="1"/>
-    <row r="640" ht="15.75" customHeight="1"/>
-    <row r="641" ht="15.75" customHeight="1"/>
-    <row r="642" ht="15.75" customHeight="1"/>
-    <row r="643" ht="15.75" customHeight="1"/>
-    <row r="644" ht="15.75" customHeight="1"/>
-    <row r="645" ht="15.75" customHeight="1"/>
-    <row r="646" ht="15.75" customHeight="1"/>
-    <row r="647" ht="15.75" customHeight="1"/>
-    <row r="648" ht="15.75" customHeight="1"/>
-    <row r="649" ht="15.75" customHeight="1"/>
-    <row r="650" ht="15.75" customHeight="1"/>
-    <row r="651" ht="15.75" customHeight="1"/>
-    <row r="652" ht="15.75" customHeight="1"/>
-    <row r="653" ht="15.75" customHeight="1"/>
-    <row r="654" ht="15.75" customHeight="1"/>
-    <row r="655" ht="15.75" customHeight="1"/>
-    <row r="656" ht="15.75" customHeight="1"/>
-    <row r="657" ht="15.75" customHeight="1"/>
-    <row r="658" ht="15.75" customHeight="1"/>
-    <row r="659" ht="15.75" customHeight="1"/>
-    <row r="660" ht="15.75" customHeight="1"/>
-    <row r="661" ht="15.75" customHeight="1"/>
-    <row r="662" ht="15.75" customHeight="1"/>
-    <row r="663" ht="15.75" customHeight="1"/>
-    <row r="664" ht="15.75" customHeight="1"/>
-    <row r="665" ht="15.75" customHeight="1"/>
-    <row r="666" ht="15.75" customHeight="1"/>
-    <row r="667" ht="15.75" customHeight="1"/>
-    <row r="668" ht="15.75" customHeight="1"/>
-    <row r="669" ht="15.75" customHeight="1"/>
-    <row r="670" ht="15.75" customHeight="1"/>
-    <row r="671" ht="15.75" customHeight="1"/>
-    <row r="672" ht="15.75" customHeight="1"/>
-    <row r="673" ht="15.75" customHeight="1"/>
-    <row r="674" ht="15.75" customHeight="1"/>
-    <row r="675" ht="15.75" customHeight="1"/>
-    <row r="676" ht="15.75" customHeight="1"/>
-    <row r="677" ht="15.75" customHeight="1"/>
-    <row r="678" ht="15.75" customHeight="1"/>
-    <row r="679" ht="15.75" customHeight="1"/>
-    <row r="680" ht="15.75" customHeight="1"/>
-    <row r="681" ht="15.75" customHeight="1"/>
-    <row r="682" ht="15.75" customHeight="1"/>
-    <row r="683" ht="15.75" customHeight="1"/>
-    <row r="684" ht="15.75" customHeight="1"/>
-    <row r="685" ht="15.75" customHeight="1"/>
-    <row r="686" ht="15.75" customHeight="1"/>
-    <row r="687" ht="15.75" customHeight="1"/>
-    <row r="688" ht="15.75" customHeight="1"/>
-    <row r="689" ht="15.75" customHeight="1"/>
-    <row r="690" ht="15.75" customHeight="1"/>
-    <row r="691" ht="15.75" customHeight="1"/>
-    <row r="692" ht="15.75" customHeight="1"/>
-    <row r="693" ht="15.75" customHeight="1"/>
-    <row r="694" ht="15.75" customHeight="1"/>
-    <row r="695" ht="15.75" customHeight="1"/>
-    <row r="696" ht="15.75" customHeight="1"/>
-    <row r="697" ht="15.75" customHeight="1"/>
-    <row r="698" ht="15.75" customHeight="1"/>
-    <row r="699" ht="15.75" customHeight="1"/>
-    <row r="700" ht="15.75" customHeight="1"/>
-    <row r="701" ht="15.75" customHeight="1"/>
-    <row r="702" ht="15.75" customHeight="1"/>
-    <row r="703" ht="15.75" customHeight="1"/>
-    <row r="704" ht="15.75" customHeight="1"/>
-    <row r="705" ht="15.75" customHeight="1"/>
-    <row r="706" ht="15.75" customHeight="1"/>
-    <row r="707" ht="15.75" customHeight="1"/>
-    <row r="708" ht="15.75" customHeight="1"/>
-    <row r="709" ht="15.75" customHeight="1"/>
-    <row r="710" ht="15.75" customHeight="1"/>
-    <row r="711" ht="15.75" customHeight="1"/>
-    <row r="712" ht="15.75" customHeight="1"/>
-    <row r="713" ht="15.75" customHeight="1"/>
-    <row r="714" ht="15.75" customHeight="1"/>
-    <row r="715" ht="15.75" customHeight="1"/>
-    <row r="716" ht="15.75" customHeight="1"/>
-    <row r="717" ht="15.75" customHeight="1"/>
-    <row r="718" ht="15.75" customHeight="1"/>
-    <row r="719" ht="15.75" customHeight="1"/>
-    <row r="720" ht="15.75" customHeight="1"/>
-    <row r="721" ht="15.75" customHeight="1"/>
-    <row r="722" ht="15.75" customHeight="1"/>
-    <row r="723" ht="15.75" customHeight="1"/>
-    <row r="724" ht="15.75" customHeight="1"/>
-    <row r="725" ht="15.75" customHeight="1"/>
-    <row r="726" ht="15.75" customHeight="1"/>
-    <row r="727" ht="15.75" customHeight="1"/>
-    <row r="728" ht="15.75" customHeight="1"/>
-    <row r="729" ht="15.75" customHeight="1"/>
-    <row r="730" ht="15.75" customHeight="1"/>
-    <row r="731" ht="15.75" customHeight="1"/>
-    <row r="732" ht="15.75" customHeight="1"/>
-    <row r="733" ht="15.75" customHeight="1"/>
-    <row r="734" ht="15.75" customHeight="1"/>
-    <row r="735" ht="15.75" customHeight="1"/>
-    <row r="736" ht="15.75" customHeight="1"/>
-    <row r="737" ht="15.75" customHeight="1"/>
-    <row r="738" ht="15.75" customHeight="1"/>
-    <row r="739" ht="15.75" customHeight="1"/>
-    <row r="740" ht="15.75" customHeight="1"/>
-    <row r="741" ht="15.75" customHeight="1"/>
-    <row r="742" ht="15.75" customHeight="1"/>
-    <row r="743" ht="15.75" customHeight="1"/>
-    <row r="744" ht="15.75" customHeight="1"/>
-    <row r="745" ht="15.75" customHeight="1"/>
-    <row r="746" ht="15.75" customHeight="1"/>
-    <row r="747" ht="15.75" customHeight="1"/>
-    <row r="748" ht="15.75" customHeight="1"/>
-    <row r="749" ht="15.75" customHeight="1"/>
-    <row r="750" ht="15.75" customHeight="1"/>
-    <row r="751" ht="15.75" customHeight="1"/>
-    <row r="752" ht="15.75" customHeight="1"/>
-    <row r="753" ht="15.75" customHeight="1"/>
-    <row r="754" ht="15.75" customHeight="1"/>
-    <row r="755" ht="15.75" customHeight="1"/>
-    <row r="756" ht="15.75" customHeight="1"/>
-    <row r="757" ht="15.75" customHeight="1"/>
-    <row r="758" ht="15.75" customHeight="1"/>
-    <row r="759" ht="15.75" customHeight="1"/>
-    <row r="760" ht="15.75" customHeight="1"/>
-    <row r="761" ht="15.75" customHeight="1"/>
-    <row r="762" ht="15.75" customHeight="1"/>
-    <row r="763" ht="15.75" customHeight="1"/>
-    <row r="764" ht="15.75" customHeight="1"/>
-    <row r="765" ht="15.75" customHeight="1"/>
-    <row r="766" ht="15.75" customHeight="1"/>
-    <row r="767" ht="15.75" customHeight="1"/>
-    <row r="768" ht="15.75" customHeight="1"/>
-    <row r="769" ht="15.75" customHeight="1"/>
-    <row r="770" ht="15.75" customHeight="1"/>
-    <row r="771" ht="15.75" customHeight="1"/>
-    <row r="772" ht="15.75" customHeight="1"/>
-    <row r="773" ht="15.75" customHeight="1"/>
-    <row r="774" ht="15.75" customHeight="1"/>
-    <row r="775" ht="15.75" customHeight="1"/>
-    <row r="776" ht="15.75" customHeight="1"/>
-    <row r="777" ht="15.75" customHeight="1"/>
-    <row r="778" ht="15.75" customHeight="1"/>
-    <row r="779" ht="15.75" customHeight="1"/>
-    <row r="780" ht="15.75" customHeight="1"/>
-    <row r="781" ht="15.75" customHeight="1"/>
-    <row r="782" ht="15.75" customHeight="1"/>
-    <row r="783" ht="15.75" customHeight="1"/>
-    <row r="784" ht="15.75" customHeight="1"/>
-    <row r="785" ht="15.75" customHeight="1"/>
-    <row r="786" ht="15.75" customHeight="1"/>
-    <row r="787" ht="15.75" customHeight="1"/>
-    <row r="788" ht="15.75" customHeight="1"/>
-    <row r="789" ht="15.75" customHeight="1"/>
-    <row r="790" ht="15.75" customHeight="1"/>
-    <row r="791" ht="15.75" customHeight="1"/>
-    <row r="792" ht="15.75" customHeight="1"/>
-    <row r="793" ht="15.75" customHeight="1"/>
-    <row r="794" ht="15.75" customHeight="1"/>
-    <row r="795" ht="15.75" customHeight="1"/>
-    <row r="796" ht="15.75" customHeight="1"/>
-    <row r="797" ht="15.75" customHeight="1"/>
-    <row r="798" ht="15.75" customHeight="1"/>
-    <row r="799" ht="15.75" customHeight="1"/>
-    <row r="800" ht="15.75" customHeight="1"/>
-    <row r="801" ht="15.75" customHeight="1"/>
-    <row r="802" ht="15.75" customHeight="1"/>
-    <row r="803" ht="15.75" customHeight="1"/>
-    <row r="804" ht="15.75" customHeight="1"/>
-    <row r="805" ht="15.75" customHeight="1"/>
-    <row r="806" ht="15.75" customHeight="1"/>
-    <row r="807" ht="15.75" customHeight="1"/>
-    <row r="808" ht="15.75" customHeight="1"/>
-    <row r="809" ht="15.75" customHeight="1"/>
-    <row r="810" ht="15.75" customHeight="1"/>
-    <row r="811" ht="15.75" customHeight="1"/>
-    <row r="812" ht="15.75" customHeight="1"/>
-    <row r="813" ht="15.75" customHeight="1"/>
-    <row r="814" ht="15.75" customHeight="1"/>
-    <row r="815" ht="15.75" customHeight="1"/>
-    <row r="816" ht="15.75" customHeight="1"/>
-    <row r="817" ht="15.75" customHeight="1"/>
-    <row r="818" ht="15.75" customHeight="1"/>
-    <row r="819" ht="15.75" customHeight="1"/>
-    <row r="820" ht="15.75" customHeight="1"/>
-    <row r="821" ht="15.75" customHeight="1"/>
-    <row r="822" ht="15.75" customHeight="1"/>
-    <row r="823" ht="15.75" customHeight="1"/>
-    <row r="824" ht="15.75" customHeight="1"/>
-    <row r="825" ht="15.75" customHeight="1"/>
-    <row r="826" ht="15.75" customHeight="1"/>
-    <row r="827" ht="15.75" customHeight="1"/>
-    <row r="828" ht="15.75" customHeight="1"/>
-    <row r="829" ht="15.75" customHeight="1"/>
-    <row r="830" ht="15.75" customHeight="1"/>
-    <row r="831" ht="15.75" customHeight="1"/>
-    <row r="832" ht="15.75" customHeight="1"/>
-    <row r="833" ht="15.75" customHeight="1"/>
-    <row r="834" ht="15.75" customHeight="1"/>
-    <row r="835" ht="15.75" customHeight="1"/>
-    <row r="836" ht="15.75" customHeight="1"/>
-    <row r="837" ht="15.75" customHeight="1"/>
-    <row r="838" ht="15.75" customHeight="1"/>
-    <row r="839" ht="15.75" customHeight="1"/>
-    <row r="840" ht="15.75" customHeight="1"/>
-    <row r="841" ht="15.75" customHeight="1"/>
-    <row r="842" ht="15.75" customHeight="1"/>
-    <row r="843" ht="15.75" customHeight="1"/>
-    <row r="844" ht="15.75" customHeight="1"/>
-    <row r="845" ht="15.75" customHeight="1"/>
-    <row r="846" ht="15.75" customHeight="1"/>
-    <row r="847" ht="15.75" customHeight="1"/>
-    <row r="848" ht="15.75" customHeight="1"/>
-    <row r="849" ht="15.75" customHeight="1"/>
-    <row r="850" ht="15.75" customHeight="1"/>
-    <row r="851" ht="15.75" customHeight="1"/>
-    <row r="852" ht="15.75" customHeight="1"/>
-    <row r="853" ht="15.75" customHeight="1"/>
-    <row r="854" ht="15.75" customHeight="1"/>
-    <row r="855" ht="15.75" customHeight="1"/>
-    <row r="856" ht="15.75" customHeight="1"/>
-    <row r="857" ht="15.75" customHeight="1"/>
-    <row r="858" ht="15.75" customHeight="1"/>
-    <row r="859" ht="15.75" customHeight="1"/>
-    <row r="860" ht="15.75" customHeight="1"/>
-    <row r="861" ht="15.75" customHeight="1"/>
-    <row r="862" ht="15.75" customHeight="1"/>
-    <row r="863" ht="15.75" customHeight="1"/>
-    <row r="864" ht="15.75" customHeight="1"/>
-    <row r="865" ht="15.75" customHeight="1"/>
-    <row r="866" ht="15.75" customHeight="1"/>
-    <row r="867" ht="15.75" customHeight="1"/>
-    <row r="868" ht="15.75" customHeight="1"/>
-    <row r="869" ht="15.75" customHeight="1"/>
-    <row r="870" ht="15.75" customHeight="1"/>
-    <row r="871" ht="15.75" customHeight="1"/>
-    <row r="872" ht="15.75" customHeight="1"/>
-    <row r="873" ht="15.75" customHeight="1"/>
-    <row r="874" ht="15.75" customHeight="1"/>
-    <row r="875" ht="15.75" customHeight="1"/>
-    <row r="876" ht="15.75" customHeight="1"/>
-    <row r="877" ht="15.75" customHeight="1"/>
-    <row r="878" ht="15.75" customHeight="1"/>
-    <row r="879" ht="15.75" customHeight="1"/>
-    <row r="880" ht="15.75" customHeight="1"/>
-    <row r="881" ht="15.75" customHeight="1"/>
-    <row r="882" ht="15.75" customHeight="1"/>
-    <row r="883" ht="15.75" customHeight="1"/>
-    <row r="884" ht="15.75" customHeight="1"/>
-    <row r="885" ht="15.75" customHeight="1"/>
-    <row r="886" ht="15.75" customHeight="1"/>
-    <row r="887" ht="15.75" customHeight="1"/>
-    <row r="888" ht="15.75" customHeight="1"/>
-    <row r="889" ht="15.75" customHeight="1"/>
-    <row r="890" ht="15.75" customHeight="1"/>
-    <row r="891" ht="15.75" customHeight="1"/>
-    <row r="892" ht="15.75" customHeight="1"/>
-    <row r="893" ht="15.75" customHeight="1"/>
-    <row r="894" ht="15.75" customHeight="1"/>
-    <row r="895" ht="15.75" customHeight="1"/>
-    <row r="896" ht="15.75" customHeight="1"/>
-    <row r="897" ht="15.75" customHeight="1"/>
-    <row r="898" ht="15.75" customHeight="1"/>
-    <row r="899" ht="15.75" customHeight="1"/>
-    <row r="900" ht="15.75" customHeight="1"/>
-    <row r="901" ht="15.75" customHeight="1"/>
-    <row r="902" ht="15.75" customHeight="1"/>
-    <row r="903" ht="15.75" customHeight="1"/>
-    <row r="904" ht="15.75" customHeight="1"/>
-    <row r="905" ht="15.75" customHeight="1"/>
-    <row r="906" ht="15.75" customHeight="1"/>
-    <row r="907" ht="15.75" customHeight="1"/>
-    <row r="908" ht="15.75" customHeight="1"/>
-    <row r="909" ht="15.75" customHeight="1"/>
-    <row r="910" ht="15.75" customHeight="1"/>
-    <row r="911" ht="15.75" customHeight="1"/>
-    <row r="912" ht="15.75" customHeight="1"/>
-    <row r="913" ht="15.75" customHeight="1"/>
-    <row r="914" ht="15.75" customHeight="1"/>
-    <row r="915" ht="15.75" customHeight="1"/>
-    <row r="916" ht="15.75" customHeight="1"/>
-    <row r="917" ht="15.75" customHeight="1"/>
-    <row r="918" ht="15.75" customHeight="1"/>
-    <row r="919" ht="15.75" customHeight="1"/>
-    <row r="920" ht="15.75" customHeight="1"/>
-    <row r="921" ht="15.75" customHeight="1"/>
-    <row r="922" ht="15.75" customHeight="1"/>
-    <row r="923" ht="15.75" customHeight="1"/>
-    <row r="924" ht="15.75" customHeight="1"/>
-    <row r="925" ht="15.75" customHeight="1"/>
-    <row r="926" ht="15.75" customHeight="1"/>
-    <row r="927" ht="15.75" customHeight="1"/>
-    <row r="928" ht="15.75" customHeight="1"/>
-    <row r="929" ht="15.75" customHeight="1"/>
-    <row r="930" ht="15.75" customHeight="1"/>
-    <row r="931" ht="15.75" customHeight="1"/>
-    <row r="932" ht="15.75" customHeight="1"/>
-    <row r="933" ht="15.75" customHeight="1"/>
-    <row r="934" ht="15.75" customHeight="1"/>
-    <row r="935" ht="15.75" customHeight="1"/>
-    <row r="936" ht="15.75" customHeight="1"/>
-    <row r="937" ht="15.75" customHeight="1"/>
-    <row r="938" ht="15.75" customHeight="1"/>
-    <row r="939" ht="15.75" customHeight="1"/>
-    <row r="940" ht="15.75" customHeight="1"/>
-    <row r="941" ht="15.75" customHeight="1"/>
-    <row r="942" ht="15.75" customHeight="1"/>
-    <row r="943" ht="15.75" customHeight="1"/>
-    <row r="944" ht="15.75" customHeight="1"/>
-    <row r="945" ht="15.75" customHeight="1"/>
-    <row r="946" ht="15.75" customHeight="1"/>
-    <row r="947" ht="15.75" customHeight="1"/>
-    <row r="948" ht="15.75" customHeight="1"/>
-    <row r="949" ht="15.75" customHeight="1"/>
-    <row r="950" ht="15.75" customHeight="1"/>
-    <row r="951" ht="15.75" customHeight="1"/>
-    <row r="952" ht="15.75" customHeight="1"/>
-    <row r="953" ht="15.75" customHeight="1"/>
-    <row r="954" ht="15.75" customHeight="1"/>
-    <row r="955" ht="15.75" customHeight="1"/>
-    <row r="956" ht="15.75" customHeight="1"/>
-    <row r="957" ht="15.75" customHeight="1"/>
-    <row r="958" ht="15.75" customHeight="1"/>
-    <row r="959" ht="15.75" customHeight="1"/>
-    <row r="960" ht="15.75" customHeight="1"/>
-    <row r="961" ht="15.75" customHeight="1"/>
-    <row r="962" ht="15.75" customHeight="1"/>
-    <row r="963" ht="15.75" customHeight="1"/>
-    <row r="964" ht="15.75" customHeight="1"/>
-    <row r="965" ht="15.75" customHeight="1"/>
-    <row r="966" ht="15.75" customHeight="1"/>
-    <row r="967" ht="15.75" customHeight="1"/>
-    <row r="968" ht="15.75" customHeight="1"/>
-    <row r="969" ht="15.75" customHeight="1"/>
-    <row r="970" ht="15.75" customHeight="1"/>
-    <row r="971" ht="15.75" customHeight="1"/>
-    <row r="972" ht="15.75" customHeight="1"/>
-    <row r="973" ht="15.75" customHeight="1"/>
-    <row r="974" ht="15.75" customHeight="1"/>
-    <row r="975" ht="15.75" customHeight="1"/>
-    <row r="976" ht="15.75" customHeight="1"/>
-    <row r="977" ht="15.75" customHeight="1"/>
-    <row r="978" ht="15.75" customHeight="1"/>
-    <row r="979" ht="15.75" customHeight="1"/>
-    <row r="980" ht="15.75" customHeight="1"/>
-    <row r="981" ht="15.75" customHeight="1"/>
-    <row r="982" ht="15.75" customHeight="1"/>
-    <row r="983" ht="15.75" customHeight="1"/>
-    <row r="984" ht="15.75" customHeight="1"/>
-    <row r="985" ht="15.75" customHeight="1"/>
-    <row r="986" ht="15.75" customHeight="1"/>
-    <row r="987" ht="15.75" customHeight="1"/>
-    <row r="988" ht="15.75" customHeight="1"/>
-    <row r="989" ht="15.75" customHeight="1"/>
-    <row r="990" ht="15.75" customHeight="1"/>
-    <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Cronograma de SC014 terminada
</commit_message>
<xml_diff>
--- a/Desarrollo/SGDS/Gestion/SGDS-CP.xlsx
+++ b/Desarrollo/SGDS/Gestion/SGDS-CP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Proyecto_Grupo_5\QuantumAnts-Software\Desarrollo\SGDS\Gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF217E9-C429-4C30-87FE-7F076AB73B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE493AB-0A58-4C0D-8628-10A16793DB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma #1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="184">
   <si>
     <t>CRONOGRAMA DEL PROYECTO</t>
   </si>
@@ -638,9 +638,6 @@
     <t>Actualizar el Documento de Guia de Estilos</t>
   </si>
   <si>
-    <t>Actualizar el Documento de Especificación de la Base de Datos</t>
-  </si>
-  <si>
     <t>Actualizar el Documento del Requisito 08: Registro de donante</t>
   </si>
   <si>
@@ -650,18 +647,6 @@
     <t>Saavedra M. (JP/AS)</t>
   </si>
   <si>
-    <t>Proceso de Script 1</t>
-  </si>
-  <si>
-    <t>Proceso de Script 2</t>
-  </si>
-  <si>
-    <t>Proceso de Script 3</t>
-  </si>
-  <si>
-    <t>Actualización de la Base de Datos</t>
-  </si>
-  <si>
     <t>Implemenctación de la Interfaz Web</t>
   </si>
   <si>
@@ -681,6 +666,18 @@
   </si>
   <si>
     <t>SGDS-ACP-SC014.DOCX</t>
+  </si>
+  <si>
+    <t>Verificación de la Base de Datos</t>
+  </si>
+  <si>
+    <t>Verificación de la Base de Datos 01</t>
+  </si>
+  <si>
+    <t>Quispe C. (T)/Sanchez W.(DBA)</t>
+  </si>
+  <si>
+    <t>Chuquispuma (PF)./Saavedra M.(JP)</t>
   </si>
 </sst>
 </file>
@@ -1447,7 +1444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1652,15 +1649,9 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1684,21 +1675,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1713,6 +1689,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1935,14 +1926,14 @@
   </sheetPr>
   <dimension ref="A1:K998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="62.42578125" customWidth="1"/>
+    <col min="2" max="2" width="72.28515625" customWidth="1"/>
     <col min="3" max="3" width="52.140625" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" customWidth="1"/>
     <col min="5" max="5" width="81.5703125" customWidth="1"/>
@@ -1953,23 +1944,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="32.25" customHeight="1">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="113" t="s">
+      <c r="B2" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="114"/>
+      <c r="C2" s="107"/>
       <c r="D2" s="2"/>
       <c r="E2" s="1"/>
       <c r="F2" s="3"/>
@@ -2159,7 +2150,7 @@
       <c r="H12" s="20">
         <v>1</v>
       </c>
-      <c r="I12" s="110" t="s">
+      <c r="I12" s="103" t="s">
         <v>24</v>
       </c>
       <c r="J12" s="2"/>
@@ -2188,7 +2179,7 @@
       <c r="H13" s="20">
         <v>1</v>
       </c>
-      <c r="I13" s="111"/>
+      <c r="I13" s="104"/>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
@@ -2214,7 +2205,7 @@
       <c r="H14" s="20">
         <v>1</v>
       </c>
-      <c r="I14" s="111"/>
+      <c r="I14" s="104"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
@@ -2240,7 +2231,7 @@
       <c r="H15" s="20">
         <v>1</v>
       </c>
-      <c r="I15" s="111"/>
+      <c r="I15" s="104"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
@@ -2267,7 +2258,7 @@
       <c r="H16" s="20">
         <v>1</v>
       </c>
-      <c r="I16" s="111"/>
+      <c r="I16" s="104"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
@@ -2294,7 +2285,7 @@
       <c r="H17" s="20">
         <v>1</v>
       </c>
-      <c r="I17" s="111"/>
+      <c r="I17" s="104"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
@@ -2321,7 +2312,7 @@
       <c r="H18" s="20">
         <v>1</v>
       </c>
-      <c r="I18" s="111"/>
+      <c r="I18" s="104"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
@@ -2348,7 +2339,7 @@
       <c r="H19" s="20">
         <v>1</v>
       </c>
-      <c r="I19" s="111"/>
+      <c r="I19" s="104"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
@@ -2375,7 +2366,7 @@
       <c r="H20" s="20">
         <v>1</v>
       </c>
-      <c r="I20" s="111"/>
+      <c r="I20" s="104"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
@@ -2402,7 +2393,7 @@
       <c r="H21" s="20">
         <v>1</v>
       </c>
-      <c r="I21" s="111"/>
+      <c r="I21" s="104"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
@@ -2429,7 +2420,7 @@
       <c r="H22" s="20">
         <v>1</v>
       </c>
-      <c r="I22" s="111"/>
+      <c r="I22" s="104"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
@@ -2456,7 +2447,7 @@
       <c r="H23" s="20">
         <v>1</v>
       </c>
-      <c r="I23" s="111"/>
+      <c r="I23" s="104"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
@@ -2537,7 +2528,7 @@
       <c r="H26" s="20">
         <v>1</v>
       </c>
-      <c r="I26" s="110" t="s">
+      <c r="I26" s="103" t="s">
         <v>62</v>
       </c>
       <c r="J26" s="2"/>
@@ -2566,7 +2557,7 @@
       <c r="H27" s="20">
         <v>1</v>
       </c>
-      <c r="I27" s="111"/>
+      <c r="I27" s="104"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
@@ -2593,7 +2584,7 @@
       <c r="H28" s="20">
         <v>1</v>
       </c>
-      <c r="I28" s="110" t="s">
+      <c r="I28" s="103" t="s">
         <v>68</v>
       </c>
       <c r="J28" s="2"/>
@@ -2622,7 +2613,7 @@
       <c r="H29" s="20">
         <v>1</v>
       </c>
-      <c r="I29" s="111"/>
+      <c r="I29" s="104"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
@@ -2646,7 +2637,7 @@
         <f>SUM(H10:H29)/20</f>
         <v>1</v>
       </c>
-      <c r="I30" s="111"/>
+      <c r="I30" s="104"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A31" s="9"/>
@@ -2835,7 +2826,7 @@
       <c r="H37" s="45">
         <v>1</v>
       </c>
-      <c r="I37" s="110" t="s">
+      <c r="I37" s="103" t="s">
         <v>78</v>
       </c>
       <c r="J37" s="46"/>
@@ -2864,7 +2855,7 @@
       <c r="H38" s="45">
         <v>1</v>
       </c>
-      <c r="I38" s="111"/>
+      <c r="I38" s="104"/>
       <c r="J38" s="46"/>
       <c r="K38" s="2"/>
     </row>
@@ -2888,7 +2879,7 @@
         <f>SUM(H31:H38)/8</f>
         <v>1</v>
       </c>
-      <c r="I39" s="111"/>
+      <c r="I39" s="104"/>
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A40" s="9"/>
@@ -3156,7 +3147,7 @@
       <c r="H49" s="52">
         <v>1</v>
       </c>
-      <c r="I49" s="110" t="s">
+      <c r="I49" s="103" t="s">
         <v>85</v>
       </c>
       <c r="J49" s="46"/>
@@ -3185,7 +3176,7 @@
       <c r="H50" s="52">
         <v>1</v>
       </c>
-      <c r="I50" s="111"/>
+      <c r="I50" s="104"/>
       <c r="J50" s="46"/>
       <c r="K50" s="2"/>
     </row>
@@ -3212,7 +3203,7 @@
       <c r="H51" s="52">
         <v>1</v>
       </c>
-      <c r="I51" s="110" t="s">
+      <c r="I51" s="103" t="s">
         <v>87</v>
       </c>
       <c r="J51" s="46"/>
@@ -3241,7 +3232,7 @@
       <c r="H52" s="52">
         <v>1</v>
       </c>
-      <c r="I52" s="111"/>
+      <c r="I52" s="104"/>
       <c r="J52" s="46"/>
       <c r="K52" s="2"/>
     </row>
@@ -3267,7 +3258,7 @@
         <f>SUM(H40:H52)/13</f>
         <v>1</v>
       </c>
-      <c r="I53" s="111"/>
+      <c r="I53" s="104"/>
     </row>
     <row r="54" spans="1:11" ht="15.75" customHeight="1">
       <c r="B54" s="22"/>
@@ -5051,16 +5042,16 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="62.42578125" customWidth="1"/>
+    <col min="2" max="2" width="66.7109375" customWidth="1"/>
     <col min="3" max="3" width="52.140625" customWidth="1"/>
     <col min="4" max="4" width="26.42578125" customWidth="1"/>
     <col min="5" max="5" width="81.5703125" customWidth="1"/>
@@ -5070,23 +5061,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="105" t="s">
         <v>165</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1"/>
-      <c r="B2" s="113" t="s">
+      <c r="B2" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="114"/>
+      <c r="C2" s="107"/>
       <c r="D2" s="2"/>
       <c r="E2" s="1"/>
       <c r="F2" s="3"/>
@@ -5203,22 +5194,22 @@
         <v>166</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>183</v>
-      </c>
-      <c r="D10" s="104" t="s">
-        <v>182</v>
-      </c>
-      <c r="E10" s="95" t="s">
-        <v>173</v>
-      </c>
-      <c r="F10" s="99">
+        <v>178</v>
+      </c>
+      <c r="D10" s="102" t="s">
+        <v>177</v>
+      </c>
+      <c r="E10" s="94" t="s">
+        <v>172</v>
+      </c>
+      <c r="F10" s="97">
         <f>C6</f>
         <v>45107</v>
       </c>
-      <c r="G10" s="99">
+      <c r="G10" s="97">
         <v>45107</v>
       </c>
-      <c r="H10" s="103">
+      <c r="H10" s="101">
         <v>1</v>
       </c>
     </row>
@@ -5230,43 +5221,43 @@
       <c r="C11" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="104" t="s">
+      <c r="D11" s="102" t="s">
         <v>118</v>
       </c>
-      <c r="E11" s="95" t="s">
-        <v>173</v>
-      </c>
-      <c r="F11" s="99">
+      <c r="E11" s="94" t="s">
+        <v>172</v>
+      </c>
+      <c r="F11" s="97">
         <v>45107</v>
       </c>
-      <c r="G11" s="98">
+      <c r="G11" s="96">
         <v>45108</v>
       </c>
-      <c r="H11" s="103">
+      <c r="H11" s="101">
         <v>0.8</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" thickBot="1">
       <c r="A12" s="9"/>
       <c r="B12" s="89" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C12" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="104" t="s">
+      <c r="D12" s="102" t="s">
         <v>156</v>
       </c>
       <c r="E12" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="99">
+      <c r="F12" s="97">
         <v>45108</v>
       </c>
-      <c r="G12" s="100">
+      <c r="G12" s="98">
         <v>45108</v>
       </c>
-      <c r="H12" s="103"/>
+      <c r="H12" s="101"/>
     </row>
     <row r="13" spans="1:8" ht="15" thickBot="1">
       <c r="A13" s="9"/>
@@ -5276,283 +5267,279 @@
       <c r="C13" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="104" t="s">
+      <c r="D13" s="102" t="s">
         <v>108</v>
       </c>
-      <c r="E13" s="95" t="s">
-        <v>173</v>
-      </c>
-      <c r="F13" s="99">
+      <c r="E13" s="94" t="s">
+        <v>172</v>
+      </c>
+      <c r="F13" s="97">
         <v>45108</v>
       </c>
-      <c r="G13" s="100">
+      <c r="G13" s="98">
         <v>45108</v>
       </c>
-      <c r="H13" s="103"/>
+      <c r="H13" s="101"/>
     </row>
     <row r="14" spans="1:8" ht="15" thickBot="1">
       <c r="A14" s="9"/>
       <c r="B14" s="89" t="s">
-        <v>170</v>
-      </c>
-      <c r="C14" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="104" t="s">
-        <v>109</v>
-      </c>
-      <c r="E14" s="96" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="99">
+        <v>171</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="102" t="s">
+        <v>119</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="97">
         <v>45108</v>
       </c>
-      <c r="G14" s="100">
+      <c r="G14" s="98">
         <v>45108</v>
       </c>
-      <c r="H14" s="103"/>
-    </row>
-    <row r="15" spans="1:8" ht="15" thickBot="1">
+      <c r="H14" s="101"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
       <c r="A15" s="9"/>
       <c r="B15" s="89" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="104" t="s">
-        <v>119</v>
+        <v>64</v>
+      </c>
+      <c r="D15" s="102" t="s">
+        <v>135</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="99">
+        <v>65</v>
+      </c>
+      <c r="F15" s="97">
         <v>45108</v>
       </c>
-      <c r="G15" s="100">
+      <c r="G15" s="98">
         <v>45108</v>
       </c>
-      <c r="H15" s="103"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A16" s="9"/>
-      <c r="B16" s="89" t="s">
-        <v>169</v>
-      </c>
-      <c r="C16" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="104" t="s">
-        <v>135</v>
-      </c>
-      <c r="E16" s="29" t="s">
+      <c r="H15" s="101"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A16" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="39"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="41">
+        <v>45107</v>
+      </c>
+      <c r="G16" s="41">
+        <v>45108</v>
+      </c>
+      <c r="H16" s="42">
+        <f>SUM(H10:H15)/7</f>
+        <v>0.25714285714285717</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15" thickBot="1">
+      <c r="A17" s="9"/>
+      <c r="B17" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="44" t="s">
+        <v>143</v>
+      </c>
+      <c r="D17" s="110" t="s">
+        <v>150</v>
+      </c>
+      <c r="E17" s="95" t="s">
         <v>65</v>
       </c>
-      <c r="F16" s="99">
-        <v>45108</v>
-      </c>
-      <c r="G16" s="100">
-        <v>45108</v>
-      </c>
-      <c r="H16" s="103"/>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A17" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="78"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="41">
-        <v>45107</v>
-      </c>
-      <c r="G17" s="41">
-        <v>45108</v>
-      </c>
-      <c r="H17" s="42">
-        <f>SUM(H10:H16)/7</f>
-        <v>0.25714285714285717</v>
-      </c>
+      <c r="F17" s="99">
+        <v>45109</v>
+      </c>
+      <c r="G17" s="99">
+        <v>45110</v>
+      </c>
+      <c r="H17" s="100"/>
     </row>
     <row r="18" spans="1:8" ht="15" thickBot="1">
       <c r="A18" s="9"/>
-      <c r="B18" s="91" t="s">
-        <v>177</v>
+      <c r="B18" s="43" t="s">
+        <v>76</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>158</v>
-      </c>
-      <c r="D18" s="107" t="s">
-        <v>131</v>
-      </c>
-      <c r="E18" s="96" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="101">
+        <v>144</v>
+      </c>
+      <c r="D18" s="110" t="s">
+        <v>151</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="F18" s="99">
         <v>45109</v>
       </c>
-      <c r="G18" s="101">
-        <v>45109</v>
-      </c>
-      <c r="H18" s="102"/>
+      <c r="G18" s="99">
+        <v>45110</v>
+      </c>
+      <c r="H18" s="100"/>
     </row>
     <row r="19" spans="1:8" ht="15" thickBot="1">
       <c r="A19" s="9"/>
-      <c r="B19" s="91" t="s">
-        <v>174</v>
-      </c>
-      <c r="C19" s="94"/>
-      <c r="D19" s="105"/>
-      <c r="E19" s="95"/>
-      <c r="F19" s="101">
+      <c r="B19" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="D19" s="110" t="s">
+        <v>156</v>
+      </c>
+      <c r="E19" s="114" t="s">
+        <v>182</v>
+      </c>
+      <c r="F19" s="99">
         <v>45109</v>
       </c>
-      <c r="G19" s="101">
-        <v>45109</v>
-      </c>
-      <c r="H19" s="102"/>
+      <c r="G19" s="99">
+        <v>45110</v>
+      </c>
+      <c r="H19" s="100"/>
     </row>
     <row r="20" spans="1:8" ht="15" thickBot="1">
       <c r="A20" s="9"/>
       <c r="B20" s="91" t="s">
-        <v>175</v>
-      </c>
-      <c r="C20" s="94"/>
-      <c r="D20" s="105"/>
-      <c r="E20" s="95"/>
-      <c r="F20" s="101">
+        <v>180</v>
+      </c>
+      <c r="C20" s="44" t="s">
+        <v>181</v>
+      </c>
+      <c r="D20" s="110" t="s">
+        <v>131</v>
+      </c>
+      <c r="E20" s="113" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="99">
         <v>45109</v>
       </c>
-      <c r="G20" s="101">
-        <v>45109</v>
-      </c>
-      <c r="H20" s="102"/>
+      <c r="G20" s="99">
+        <v>45110</v>
+      </c>
+      <c r="H20" s="100"/>
     </row>
     <row r="21" spans="1:8" ht="15" thickBot="1">
       <c r="A21" s="9"/>
       <c r="B21" s="91" t="s">
-        <v>176</v>
-      </c>
-      <c r="C21" s="94"/>
-      <c r="D21" s="106"/>
-      <c r="E21" s="96"/>
-      <c r="F21" s="101">
+        <v>173</v>
+      </c>
+      <c r="C21" s="47" t="s">
+        <v>148</v>
+      </c>
+      <c r="D21" s="111" t="s">
+        <v>164</v>
+      </c>
+      <c r="E21" s="95" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="99">
         <v>45109</v>
       </c>
-      <c r="G21" s="101">
+      <c r="G21" s="99">
         <v>45110</v>
       </c>
-      <c r="H21" s="102"/>
+      <c r="H21" s="100"/>
     </row>
     <row r="22" spans="1:8" ht="15" thickBot="1">
       <c r="A22" s="9"/>
-      <c r="B22" s="91" t="s">
-        <v>178</v>
+      <c r="B22" s="89" t="s">
+        <v>84</v>
       </c>
       <c r="C22" s="47" t="s">
-        <v>148</v>
-      </c>
-      <c r="D22" s="108" t="s">
-        <v>164</v>
-      </c>
-      <c r="E22" s="97" t="s">
+        <v>159</v>
+      </c>
+      <c r="D22" s="110" t="s">
+        <v>175</v>
+      </c>
+      <c r="E22" s="95" t="s">
         <v>61</v>
       </c>
-      <c r="F22" s="101">
-        <v>45109</v>
-      </c>
-      <c r="G22" s="101">
+      <c r="F22" s="99">
         <v>45111</v>
       </c>
-      <c r="H22" s="102"/>
+      <c r="G22" s="99">
+        <v>45111</v>
+      </c>
+      <c r="H22" s="100"/>
     </row>
     <row r="23" spans="1:8" ht="15" thickBot="1">
       <c r="A23" s="9"/>
-      <c r="B23" s="89" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" s="47" t="s">
-        <v>159</v>
-      </c>
-      <c r="D23" s="107" t="s">
-        <v>180</v>
-      </c>
-      <c r="E23" s="97" t="s">
-        <v>61</v>
-      </c>
-      <c r="F23" s="101">
+      <c r="B23" s="92" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="112" t="s">
+        <v>162</v>
+      </c>
+      <c r="E23" s="95" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" s="99">
         <v>45111</v>
       </c>
-      <c r="G23" s="101">
+      <c r="G23" s="99">
         <v>45111</v>
       </c>
-      <c r="H23" s="102"/>
+      <c r="H23" s="100"/>
     </row>
     <row r="24" spans="1:8" ht="15" thickBot="1">
       <c r="A24" s="9"/>
-      <c r="B24" s="92" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="109" t="s">
-        <v>162</v>
-      </c>
-      <c r="E24" s="97" t="s">
-        <v>65</v>
-      </c>
-      <c r="F24" s="101">
-        <v>45111</v>
-      </c>
-      <c r="G24" s="101">
-        <v>45111</v>
-      </c>
-      <c r="H24" s="102"/>
-    </row>
-    <row r="25" spans="1:8" ht="15" thickBot="1">
-      <c r="A25" s="9"/>
-      <c r="B25" s="93" t="s">
+      <c r="B24" s="93" t="s">
+        <v>174</v>
+      </c>
+      <c r="C24" s="59" t="s">
+        <v>176</v>
+      </c>
+      <c r="D24" s="110" t="s">
         <v>179</v>
       </c>
-      <c r="C25" s="59" t="s">
-        <v>181</v>
-      </c>
-      <c r="D25" s="107" t="s">
-        <v>184</v>
-      </c>
-      <c r="E25" s="95" t="s">
+      <c r="E24" s="94" t="s">
         <v>48</v>
       </c>
-      <c r="F25" s="101">
+      <c r="F24" s="99">
         <v>45112</v>
       </c>
-      <c r="G25" s="101">
+      <c r="G24" s="99">
         <v>45112</v>
       </c>
-      <c r="H25" s="102"/>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A26" s="37" t="s">
+      <c r="H24" s="100"/>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A25" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="38" t="s">
+      <c r="B25" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="86"/>
-      <c r="D26" s="78"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="55">
+      <c r="C25" s="86"/>
+      <c r="D25" s="78"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="55">
         <v>45109</v>
       </c>
-      <c r="G26" s="41">
+      <c r="G25" s="41">
         <v>45112</v>
       </c>
-      <c r="H26" s="56">
-        <f>SUM(H18:H25)/8</f>
+      <c r="H25" s="56">
+        <f>SUM(H17:H24)/8</f>
         <v>0</v>
       </c>
     </row>
@@ -5562,7 +5549,7 @@
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D24" r:id="rId1" display="http://sgds.rds-02.py/" xr:uid="{9B119A75-9F9D-420B-A8DA-DC877DBFE7BA}"/>
+    <hyperlink ref="D23" r:id="rId1" display="http://sgds.rds-02.py/" xr:uid="{9B119A75-9F9D-420B-A8DA-DC877DBFE7BA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5596,10 +5583,10 @@
       <c r="C2" s="9"/>
     </row>
     <row r="3" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="108" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="116"/>
+      <c r="C3" s="109"/>
     </row>
     <row r="4" spans="2:3" ht="15.75" customHeight="1">
       <c r="B4" s="68" t="s">

</xml_diff>

<commit_message>
SGDS-DAS01 actualizado y cronograma actualizado
</commit_message>
<xml_diff>
--- a/Desarrollo/SGDS/Gestion/SGDS-CP.xlsx
+++ b/Desarrollo/SGDS/Gestion/SGDS-CP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Proyecto_Grupo_5\QuantumAnts-Software\Desarrollo\SGDS\Gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE493AB-0A58-4C0D-8628-10A16793DB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E84955B-5537-4836-AFB4-20358634E204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1676,6 +1676,21 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1689,21 +1704,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1944,23 +1944,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="32.25" customHeight="1">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="110" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
-      <c r="H1" s="104"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="107"/>
+      <c r="C2" s="112"/>
       <c r="D2" s="2"/>
       <c r="E2" s="1"/>
       <c r="F2" s="3"/>
@@ -2150,7 +2150,7 @@
       <c r="H12" s="20">
         <v>1</v>
       </c>
-      <c r="I12" s="103" t="s">
+      <c r="I12" s="108" t="s">
         <v>24</v>
       </c>
       <c r="J12" s="2"/>
@@ -2179,7 +2179,7 @@
       <c r="H13" s="20">
         <v>1</v>
       </c>
-      <c r="I13" s="104"/>
+      <c r="I13" s="109"/>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
@@ -2205,7 +2205,7 @@
       <c r="H14" s="20">
         <v>1</v>
       </c>
-      <c r="I14" s="104"/>
+      <c r="I14" s="109"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
@@ -2231,7 +2231,7 @@
       <c r="H15" s="20">
         <v>1</v>
       </c>
-      <c r="I15" s="104"/>
+      <c r="I15" s="109"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
@@ -2258,7 +2258,7 @@
       <c r="H16" s="20">
         <v>1</v>
       </c>
-      <c r="I16" s="104"/>
+      <c r="I16" s="109"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
@@ -2285,7 +2285,7 @@
       <c r="H17" s="20">
         <v>1</v>
       </c>
-      <c r="I17" s="104"/>
+      <c r="I17" s="109"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
@@ -2312,7 +2312,7 @@
       <c r="H18" s="20">
         <v>1</v>
       </c>
-      <c r="I18" s="104"/>
+      <c r="I18" s="109"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
@@ -2339,7 +2339,7 @@
       <c r="H19" s="20">
         <v>1</v>
       </c>
-      <c r="I19" s="104"/>
+      <c r="I19" s="109"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
@@ -2366,7 +2366,7 @@
       <c r="H20" s="20">
         <v>1</v>
       </c>
-      <c r="I20" s="104"/>
+      <c r="I20" s="109"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
@@ -2393,7 +2393,7 @@
       <c r="H21" s="20">
         <v>1</v>
       </c>
-      <c r="I21" s="104"/>
+      <c r="I21" s="109"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
@@ -2420,7 +2420,7 @@
       <c r="H22" s="20">
         <v>1</v>
       </c>
-      <c r="I22" s="104"/>
+      <c r="I22" s="109"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
@@ -2447,7 +2447,7 @@
       <c r="H23" s="20">
         <v>1</v>
       </c>
-      <c r="I23" s="104"/>
+      <c r="I23" s="109"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
@@ -2528,7 +2528,7 @@
       <c r="H26" s="20">
         <v>1</v>
       </c>
-      <c r="I26" s="103" t="s">
+      <c r="I26" s="108" t="s">
         <v>62</v>
       </c>
       <c r="J26" s="2"/>
@@ -2557,7 +2557,7 @@
       <c r="H27" s="20">
         <v>1</v>
       </c>
-      <c r="I27" s="104"/>
+      <c r="I27" s="109"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
@@ -2584,7 +2584,7 @@
       <c r="H28" s="20">
         <v>1</v>
       </c>
-      <c r="I28" s="103" t="s">
+      <c r="I28" s="108" t="s">
         <v>68</v>
       </c>
       <c r="J28" s="2"/>
@@ -2613,7 +2613,7 @@
       <c r="H29" s="20">
         <v>1</v>
       </c>
-      <c r="I29" s="104"/>
+      <c r="I29" s="109"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
@@ -2637,7 +2637,7 @@
         <f>SUM(H10:H29)/20</f>
         <v>1</v>
       </c>
-      <c r="I30" s="104"/>
+      <c r="I30" s="109"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A31" s="9"/>
@@ -2826,7 +2826,7 @@
       <c r="H37" s="45">
         <v>1</v>
       </c>
-      <c r="I37" s="103" t="s">
+      <c r="I37" s="108" t="s">
         <v>78</v>
       </c>
       <c r="J37" s="46"/>
@@ -2855,7 +2855,7 @@
       <c r="H38" s="45">
         <v>1</v>
       </c>
-      <c r="I38" s="104"/>
+      <c r="I38" s="109"/>
       <c r="J38" s="46"/>
       <c r="K38" s="2"/>
     </row>
@@ -2879,7 +2879,7 @@
         <f>SUM(H31:H38)/8</f>
         <v>1</v>
       </c>
-      <c r="I39" s="104"/>
+      <c r="I39" s="109"/>
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A40" s="9"/>
@@ -3147,7 +3147,7 @@
       <c r="H49" s="52">
         <v>1</v>
       </c>
-      <c r="I49" s="103" t="s">
+      <c r="I49" s="108" t="s">
         <v>85</v>
       </c>
       <c r="J49" s="46"/>
@@ -3176,7 +3176,7 @@
       <c r="H50" s="52">
         <v>1</v>
       </c>
-      <c r="I50" s="104"/>
+      <c r="I50" s="109"/>
       <c r="J50" s="46"/>
       <c r="K50" s="2"/>
     </row>
@@ -3203,7 +3203,7 @@
       <c r="H51" s="52">
         <v>1</v>
       </c>
-      <c r="I51" s="103" t="s">
+      <c r="I51" s="108" t="s">
         <v>87</v>
       </c>
       <c r="J51" s="46"/>
@@ -3232,7 +3232,7 @@
       <c r="H52" s="52">
         <v>1</v>
       </c>
-      <c r="I52" s="104"/>
+      <c r="I52" s="109"/>
       <c r="J52" s="46"/>
       <c r="K52" s="2"/>
     </row>
@@ -3258,7 +3258,7 @@
         <f>SUM(H40:H52)/13</f>
         <v>1</v>
       </c>
-      <c r="I53" s="104"/>
+      <c r="I53" s="109"/>
     </row>
     <row r="54" spans="1:11" ht="15.75" customHeight="1">
       <c r="B54" s="22"/>
@@ -5045,7 +5045,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -5061,23 +5061,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="110" t="s">
         <v>165</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
-      <c r="H1" s="104"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1"/>
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="107"/>
+      <c r="C2" s="112"/>
       <c r="D2" s="2"/>
       <c r="E2" s="1"/>
       <c r="F2" s="3"/>
@@ -5234,7 +5234,7 @@
         <v>45108</v>
       </c>
       <c r="H11" s="101">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" thickBot="1">
@@ -5279,7 +5279,9 @@
       <c r="G13" s="98">
         <v>45108</v>
       </c>
-      <c r="H13" s="101"/>
+      <c r="H13" s="101">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="15" thickBot="1">
       <c r="A14" s="9"/>
@@ -5343,7 +5345,7 @@
       </c>
       <c r="H16" s="42">
         <f>SUM(H10:H15)/7</f>
-        <v>0.25714285714285717</v>
+        <v>0.42857142857142855</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15" thickBot="1">
@@ -5354,7 +5356,7 @@
       <c r="C17" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="D17" s="110" t="s">
+      <c r="D17" s="103" t="s">
         <v>150</v>
       </c>
       <c r="E17" s="95" t="s">
@@ -5376,7 +5378,7 @@
       <c r="C18" s="44" t="s">
         <v>144</v>
       </c>
-      <c r="D18" s="110" t="s">
+      <c r="D18" s="103" t="s">
         <v>151</v>
       </c>
       <c r="E18" s="29" t="s">
@@ -5398,10 +5400,10 @@
       <c r="C19" s="44" t="s">
         <v>140</v>
       </c>
-      <c r="D19" s="110" t="s">
+      <c r="D19" s="103" t="s">
         <v>156</v>
       </c>
-      <c r="E19" s="114" t="s">
+      <c r="E19" s="107" t="s">
         <v>182</v>
       </c>
       <c r="F19" s="99">
@@ -5420,10 +5422,10 @@
       <c r="C20" s="44" t="s">
         <v>181</v>
       </c>
-      <c r="D20" s="110" t="s">
+      <c r="D20" s="103" t="s">
         <v>131</v>
       </c>
-      <c r="E20" s="113" t="s">
+      <c r="E20" s="106" t="s">
         <v>33</v>
       </c>
       <c r="F20" s="99">
@@ -5442,7 +5444,7 @@
       <c r="C21" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="D21" s="111" t="s">
+      <c r="D21" s="104" t="s">
         <v>164</v>
       </c>
       <c r="E21" s="95" t="s">
@@ -5464,7 +5466,7 @@
       <c r="C22" s="47" t="s">
         <v>159</v>
       </c>
-      <c r="D22" s="110" t="s">
+      <c r="D22" s="103" t="s">
         <v>175</v>
       </c>
       <c r="E22" s="95" t="s">
@@ -5486,7 +5488,7 @@
       <c r="C23" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="D23" s="112" t="s">
+      <c r="D23" s="105" t="s">
         <v>162</v>
       </c>
       <c r="E23" s="95" t="s">
@@ -5508,7 +5510,7 @@
       <c r="C24" s="59" t="s">
         <v>176</v>
       </c>
-      <c r="D24" s="110" t="s">
+      <c r="D24" s="103" t="s">
         <v>179</v>
       </c>
       <c r="E24" s="94" t="s">
@@ -5583,10 +5585,10 @@
       <c r="C2" s="9"/>
     </row>
     <row r="3" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B3" s="108" t="s">
+      <c r="B3" s="113" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="109"/>
+      <c r="C3" s="114"/>
     </row>
     <row r="4" spans="2:3" ht="15.75" customHeight="1">
       <c r="B4" s="68" t="s">

</xml_diff>

<commit_message>
Plan actuaizado, Acta de cierre finalizado, Cronograma actualizado
</commit_message>
<xml_diff>
--- a/Desarrollo/SGDS/Gestion/SGDS-CP.xlsx
+++ b/Desarrollo/SGDS/Gestion/SGDS-CP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\Trabajo_Max\Proyecto_Gestion\QuantumAnts-Software\Desarrollo\SGDS\Gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883C4125-2BAC-473A-AB6A-F06A77A78744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085C94F0-AEDD-47FC-91C0-3037FD6C6018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -647,9 +647,6 @@
     <t>Elaborar del acta de cierre de la solicitud del proyecto</t>
   </si>
   <si>
-    <t>SGDS-PS-SC014.py</t>
-  </si>
-  <si>
     <t>Acta de Cierre de la Solicitud de Cambio 14 del Proyecto</t>
   </si>
   <si>
@@ -659,9 +656,6 @@
     <t>Documento del Plan de la Gestión de la Configuración</t>
   </si>
   <si>
-    <t>SGDS-ACP-SC014.DOCX</t>
-  </si>
-  <si>
     <t>Verificación de la Base de Datos</t>
   </si>
   <si>
@@ -677,10 +671,16 @@
     <t>Actualizar el Documento del Requisito 08: Accesibilidad</t>
   </si>
   <si>
-    <t>CRONOGRAMA DEL PROYECTO - SC017</t>
-  </si>
-  <si>
     <t>SGDS.RDS-04.DOCX</t>
+  </si>
+  <si>
+    <t>CRONOGRAMA DEL PROYECTO - SC021</t>
+  </si>
+  <si>
+    <t>SGDS-PS-SC021.py</t>
+  </si>
+  <si>
+    <t>SGDS-ACP-SC021.DOCX</t>
   </si>
 </sst>
 </file>
@@ -1698,6 +1698,9 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="7" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1711,9 +1714,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="42" fillId="7" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1936,8 +1936,8 @@
   </sheetPr>
   <dimension ref="A1:K998"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="C38" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -1954,23 +1954,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="32.25" customHeight="1">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="110" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="108"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="110" t="s">
+      <c r="B2" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="111"/>
+      <c r="C2" s="112"/>
       <c r="D2" s="2"/>
       <c r="E2" s="1"/>
       <c r="F2" s="3"/>
@@ -2160,7 +2160,7 @@
       <c r="H12" s="20">
         <v>1</v>
       </c>
-      <c r="I12" s="107" t="s">
+      <c r="I12" s="108" t="s">
         <v>24</v>
       </c>
       <c r="J12" s="2"/>
@@ -2189,7 +2189,7 @@
       <c r="H13" s="20">
         <v>1</v>
       </c>
-      <c r="I13" s="108"/>
+      <c r="I13" s="109"/>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
@@ -2215,7 +2215,7 @@
       <c r="H14" s="20">
         <v>1</v>
       </c>
-      <c r="I14" s="108"/>
+      <c r="I14" s="109"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
@@ -2241,7 +2241,7 @@
       <c r="H15" s="20">
         <v>1</v>
       </c>
-      <c r="I15" s="108"/>
+      <c r="I15" s="109"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
@@ -2268,7 +2268,7 @@
       <c r="H16" s="20">
         <v>1</v>
       </c>
-      <c r="I16" s="108"/>
+      <c r="I16" s="109"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
@@ -2295,7 +2295,7 @@
       <c r="H17" s="20">
         <v>1</v>
       </c>
-      <c r="I17" s="108"/>
+      <c r="I17" s="109"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
@@ -2322,7 +2322,7 @@
       <c r="H18" s="20">
         <v>1</v>
       </c>
-      <c r="I18" s="108"/>
+      <c r="I18" s="109"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
@@ -2349,7 +2349,7 @@
       <c r="H19" s="20">
         <v>1</v>
       </c>
-      <c r="I19" s="108"/>
+      <c r="I19" s="109"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
@@ -2376,7 +2376,7 @@
       <c r="H20" s="20">
         <v>1</v>
       </c>
-      <c r="I20" s="108"/>
+      <c r="I20" s="109"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
@@ -2403,7 +2403,7 @@
       <c r="H21" s="20">
         <v>1</v>
       </c>
-      <c r="I21" s="108"/>
+      <c r="I21" s="109"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
@@ -2430,7 +2430,7 @@
       <c r="H22" s="20">
         <v>1</v>
       </c>
-      <c r="I22" s="108"/>
+      <c r="I22" s="109"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
@@ -2457,7 +2457,7 @@
       <c r="H23" s="20">
         <v>1</v>
       </c>
-      <c r="I23" s="108"/>
+      <c r="I23" s="109"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
@@ -2538,7 +2538,7 @@
       <c r="H26" s="20">
         <v>1</v>
       </c>
-      <c r="I26" s="107" t="s">
+      <c r="I26" s="108" t="s">
         <v>62</v>
       </c>
       <c r="J26" s="2"/>
@@ -2567,7 +2567,7 @@
       <c r="H27" s="20">
         <v>1</v>
       </c>
-      <c r="I27" s="108"/>
+      <c r="I27" s="109"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
@@ -2594,7 +2594,7 @@
       <c r="H28" s="20">
         <v>1</v>
       </c>
-      <c r="I28" s="107" t="s">
+      <c r="I28" s="108" t="s">
         <v>68</v>
       </c>
       <c r="J28" s="2"/>
@@ -2623,7 +2623,7 @@
       <c r="H29" s="20">
         <v>1</v>
       </c>
-      <c r="I29" s="108"/>
+      <c r="I29" s="109"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
@@ -2647,7 +2647,7 @@
         <f>SUM(H10:H29)/20</f>
         <v>1</v>
       </c>
-      <c r="I30" s="108"/>
+      <c r="I30" s="109"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A31" s="9"/>
@@ -2836,7 +2836,7 @@
       <c r="H37" s="45">
         <v>1</v>
       </c>
-      <c r="I37" s="107" t="s">
+      <c r="I37" s="108" t="s">
         <v>78</v>
       </c>
       <c r="J37" s="46"/>
@@ -2865,7 +2865,7 @@
       <c r="H38" s="45">
         <v>1</v>
       </c>
-      <c r="I38" s="108"/>
+      <c r="I38" s="109"/>
       <c r="J38" s="46"/>
       <c r="K38" s="2"/>
     </row>
@@ -2889,7 +2889,7 @@
         <f>SUM(H31:H38)/8</f>
         <v>1</v>
       </c>
-      <c r="I39" s="108"/>
+      <c r="I39" s="109"/>
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A40" s="9"/>
@@ -3157,7 +3157,7 @@
       <c r="H49" s="52">
         <v>1</v>
       </c>
-      <c r="I49" s="107" t="s">
+      <c r="I49" s="108" t="s">
         <v>85</v>
       </c>
       <c r="J49" s="46"/>
@@ -3186,7 +3186,7 @@
       <c r="H50" s="52">
         <v>1</v>
       </c>
-      <c r="I50" s="108"/>
+      <c r="I50" s="109"/>
       <c r="J50" s="46"/>
       <c r="K50" s="2"/>
     </row>
@@ -3213,7 +3213,7 @@
       <c r="H51" s="52">
         <v>1</v>
       </c>
-      <c r="I51" s="107" t="s">
+      <c r="I51" s="108" t="s">
         <v>87</v>
       </c>
       <c r="J51" s="46"/>
@@ -3242,7 +3242,7 @@
       <c r="H52" s="52">
         <v>1</v>
       </c>
-      <c r="I52" s="108"/>
+      <c r="I52" s="109"/>
       <c r="J52" s="46"/>
       <c r="K52" s="2"/>
     </row>
@@ -3268,7 +3268,7 @@
         <f>SUM(H40:H52)/13</f>
         <v>1</v>
       </c>
-      <c r="I53" s="108"/>
+      <c r="I53" s="109"/>
     </row>
     <row r="54" spans="1:11" ht="15.75" customHeight="1">
       <c r="B54" s="22"/>
@@ -5054,8 +5054,8 @@
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23:H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -5071,23 +5071,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25">
-      <c r="A1" s="109" t="s">
-        <v>183</v>
-      </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="108"/>
+      <c r="A1" s="110" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1"/>
-      <c r="B2" s="110" t="s">
+      <c r="B2" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="111"/>
+      <c r="C2" s="112"/>
       <c r="D2" s="2"/>
       <c r="E2" s="1"/>
       <c r="F2" s="3"/>
@@ -5204,10 +5204,10 @@
         <v>165</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D10" s="102" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E10" s="94" t="s">
         <v>170</v>
@@ -5250,7 +5250,7 @@
     <row r="12" spans="1:8" ht="15" thickBot="1">
       <c r="A12" s="9"/>
       <c r="B12" s="89" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C12" s="30" t="s">
         <v>50</v>
@@ -5400,7 +5400,7 @@
         <v>151</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F18" s="99">
         <v>45109</v>
@@ -5424,7 +5424,7 @@
         <v>156</v>
       </c>
       <c r="E19" s="106" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F19" s="99">
         <v>45109</v>
@@ -5439,10 +5439,10 @@
     <row r="20" spans="1:8" ht="15" thickBot="1">
       <c r="A20" s="9"/>
       <c r="B20" s="91" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C20" s="44" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D20" s="103" t="s">
         <v>131</v>
@@ -5493,7 +5493,7 @@
         <v>159</v>
       </c>
       <c r="D22" s="103" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="E22" s="95" t="s">
         <v>61</v>
@@ -5516,8 +5516,8 @@
       <c r="C23" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="D23" s="114" t="s">
-        <v>184</v>
+      <c r="D23" s="107" t="s">
+        <v>181</v>
       </c>
       <c r="E23" s="95" t="s">
         <v>65</v>
@@ -5538,10 +5538,10 @@
         <v>172</v>
       </c>
       <c r="C24" s="59" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D24" s="103" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="E24" s="94" t="s">
         <v>48</v>
@@ -5552,7 +5552,9 @@
       <c r="G24" s="99">
         <v>45112</v>
       </c>
-      <c r="H24" s="100"/>
+      <c r="H24" s="100">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" thickBot="1">
       <c r="A25" s="37" t="s">
@@ -5572,7 +5574,7 @@
       </c>
       <c r="H25" s="56">
         <f>SUM(H17:H24)/8</f>
-        <v>0.875</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5616,10 +5618,10 @@
       <c r="C2" s="9"/>
     </row>
     <row r="3" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B3" s="112" t="s">
+      <c r="B3" s="113" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="113"/>
+      <c r="C3" s="114"/>
     </row>
     <row r="4" spans="2:3" ht="15.75" customHeight="1">
       <c r="B4" s="68" t="s">

</xml_diff>